<commit_message>
[MINOR] Added else result to conditional tree
Former-commit-id: 997cfe4dc045dc6018da8c98ceb9b9f718025719
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Clustering.xlsx
+++ b/Docs/Content/HungryDragonContent_Clustering.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mamuela/Repository/dragon/client/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F4D051C-9013-754D-A2C9-D70CD8543D9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="15945"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cluster" sheetId="2" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="46">
   <si>
     <t>&lt;Definition&gt;</t>
   </si>
@@ -59,9 +60,6 @@
     <t>[elseTreeRule]</t>
   </si>
   <si>
-    <t>[result]</t>
-  </si>
-  <si>
     <t>CLUSTER RULE TREE</t>
   </si>
   <si>
@@ -71,9 +69,6 @@
     <t>CLUSTER_TREE_RULE_002</t>
   </si>
   <si>
-    <t>CLUSTER_001</t>
-  </si>
-  <si>
     <t>CLUSTER_RULE_002</t>
   </si>
   <si>
@@ -99,12 +94,81 @@
   </si>
   <si>
     <t>All clusters available</t>
+  </si>
+  <si>
+    <t>[thenTreeRule]</t>
+  </si>
+  <si>
+    <t>CLUSTER_RULE_003</t>
+  </si>
+  <si>
+    <t>CLUSTER_NON_PAYER</t>
+  </si>
+  <si>
+    <t>CLUSTER_RULE_004</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_RULE_003</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_RULE_004</t>
+  </si>
+  <si>
+    <t>[thenResult]</t>
+  </si>
+  <si>
+    <t>[elseResult]</t>
+  </si>
+  <si>
+    <t>CLUSTER_2</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_RULE_005</t>
+  </si>
+  <si>
+    <t>CLUSTER_RULE_005</t>
+  </si>
+  <si>
+    <t>CLUSTER_10</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_RULE_006</t>
+  </si>
+  <si>
+    <t>CLUSTER_RULE_006</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_RULE_007</t>
+  </si>
+  <si>
+    <t>score &lt; 13e+3</t>
+  </si>
+  <si>
+    <t>CLUSTER_RULE_007</t>
+  </si>
+  <si>
+    <t>CLUSTER_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model.deviceProfile == 0 || model.deviceProfile == 1  </t>
+  </si>
+  <si>
+    <t>model.score &lt; 15e+3</t>
+  </si>
+  <si>
+    <t>model.deviceProfile != 4</t>
+  </si>
+  <si>
+    <t>["GROUP_5","GROUP_6","GROUP_7","Others","Tier 1","Tier 2","Tier 3"].indexOf(model.countryGroup) &gt;= 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">["GROUP_2","GROUP_3","GROUP_4"].indexOf(model.countryGroup) &gt;=0 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -152,12 +216,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -194,14 +259,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -265,45 +324,6 @@
         <color auto="1"/>
       </right>
       <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
         <color auto="1"/>
       </top>
       <bottom/>
@@ -313,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -338,26 +358,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
-    <dxf>
+  <dxfs count="31">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -368,15 +406,211 @@
         <top style="thin">
           <color auto="1"/>
         </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -431,16 +665,16 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color auto="1"/>
-        </right>
       </border>
     </dxf>
     <dxf>
@@ -475,34 +709,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -579,16 +785,16 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color auto="1"/>
-        </right>
       </border>
     </dxf>
     <dxf>
@@ -626,6 +832,89 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -657,198 +946,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1013,49 +1110,51 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B12:D13" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26" totalsRowBorderDxfId="25">
-  <autoFilter ref="B12:D13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="gameSettings" displayName="gameSettings" ref="B15:D18" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+  <autoFilter ref="B15:D18" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{clusterTreeDefinitions}" dataDxfId="24"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="23"/>
-    <tableColumn id="3" name="[firstTreeRule]" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{clusterTreeDefinitions}" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[firstTreeRule]" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B18:F20" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="20" tableBorderDxfId="21" totalsRowBorderDxfId="19">
-  <autoFilter ref="B18:F20"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="{clusterRuleTreeDefinitions}" dataDxfId="18"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="17"/>
-    <tableColumn id="3" name="[ifRule]" dataDxfId="16"/>
-    <tableColumn id="4" name="[elseTreeRule]" dataDxfId="15"/>
-    <tableColumn id="5" name="[result]" dataDxfId="14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="B23:H30" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+  <autoFilter ref="B23:H30" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{clusterRuleTreeDefinitions}" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[ifRule]" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[thenTreeRule]" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="[elseTreeRule]" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{72690AA1-8EC8-5142-8AA4-B36115E2BB1D}" name="[thenResult]" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{EBAF7F31-0A9D-204A-A4D5-9377209DD2F4}" name="[elseResult]" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings4" displayName="gameSettings4" ref="B25:D27" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
-  <autoFilter ref="B25:D27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="gameSettings4" displayName="gameSettings4" ref="B37:D44" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+  <autoFilter ref="B37:D44" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{clusterRuleDefinitions}" dataDxfId="8"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="7"/>
-    <tableColumn id="3" name="[rule]" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="{clusterRuleDefinitions}" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="[sku]" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="[rule]" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="gameSettings45" displayName="gameSettings45" ref="B6:C7" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="3" tableBorderDxfId="4" totalsRowBorderDxfId="2">
-  <autoFilter ref="B6:C7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="gameSettings45" displayName="gameSettings45" ref="B6:C10" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+  <autoFilter ref="B6:C10" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="{clusterDefinitions}" dataDxfId="1"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="{clusterDefinitions}" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="[sku]" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1323,32 +1422,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A3:K27"/>
+  <dimension ref="A3:K44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="35.85546875" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" customWidth="1"/>
-    <col min="4" max="4" width="46.7109375" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="35.83203125" customWidth="1"/>
+    <col min="3" max="3" width="39.1640625" customWidth="1"/>
+    <col min="4" max="4" width="83" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" customWidth="1"/>
     <col min="8" max="22" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:11" ht="24" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -1360,11 +1459,11 @@
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="8"/>
       <c r="B5" s="11"/>
       <c r="C5" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="10"/>
@@ -1375,217 +1474,409 @@
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="6" spans="1:11" ht="100.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="97" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B10" s="7" t="s">
+      <c r="C7" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
+    </row>
+    <row r="12" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="B13" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="9" t="s">
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="8"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-    </row>
-    <row r="12" spans="1:11" ht="119.25" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
+      <c r="D14" s="9"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+    </row>
+    <row r="15" spans="1:11" ht="115" x14ac:dyDescent="0.2">
+      <c r="B15" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D15" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B16" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B16" s="7" t="s">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B17" s="3"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B18" s="14"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="18"/>
+    </row>
+    <row r="20" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="B21" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+    </row>
+    <row r="22" spans="2:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="B22" s="11"/>
+      <c r="C22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="8"/>
+    </row>
+    <row r="23" spans="2:11" ht="134" x14ac:dyDescent="0.2">
+      <c r="B23" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B24" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="11"/>
-      <c r="C17" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="8"/>
-    </row>
-    <row r="18" spans="1:11" ht="138.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="14" t="s">
+      <c r="E24" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="20"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="16" t="s">
+      <c r="C25" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="D25" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F19" s="17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="19"/>
-      <c r="F20" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B23" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-    </row>
-    <row r="25" spans="1:11" ht="119.25" x14ac:dyDescent="0.25">
-      <c r="B25" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E25" s="19"/>
+      <c r="F25" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" s="15"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="1" t="b">
+      <c r="C26" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="15"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B27" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B28" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B29" s="12"/>
+      <c r="C29" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H29" s="19"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B30" s="12"/>
+      <c r="C30" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="H30" s="19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="B35" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="8"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" s="9"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+    </row>
+    <row r="37" spans="1:11" ht="115" x14ac:dyDescent="0.2">
+      <c r="B37" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="21" t="s">
+      <c r="D37" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B38" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" s="1" t="b">
+      <c r="C38" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B39" s="3" t="s">
         <v>0</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B40" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B41" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B42" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B43" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B44" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D13:E13 D19:E20 D26:E26 D27 D7:E7"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D16 D17:E18 D38:E38 D7:E7 E25" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[MINOR] Added definition tag to every field
Former-commit-id: 9e0c295ed89dff075ee5502c58999134416ed2a6
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Clustering.xlsx
+++ b/Docs/Content/HungryDragonContent_Clustering.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mamuela/Repository/dragon/server/tools/scripts/clusterTreeValidator/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240A0E4E-D962-F94C-9266-323FE995E900}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cluster" sheetId="2" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="94">
   <si>
     <t>&lt;Definition&gt;</t>
   </si>
@@ -311,8 +312,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,13 +349,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -520,7 +514,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -545,18 +539,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1300,51 +1293,51 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B15:D18" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
-  <autoFilter ref="B15:D18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="gameSettings" displayName="gameSettings" ref="B15:D18" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+  <autoFilter ref="B15:D18" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{clusterTreeDefinitions}" dataDxfId="26"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="25"/>
-    <tableColumn id="3" name="[firstTreeRule]" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{clusterTreeDefinitions}" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[firstTreeRule]" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B23:H59" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
-  <autoFilter ref="B23:H59"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="B23:H59" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+  <autoFilter ref="B23:H59" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{clusterRuleTreeDefinitions}" dataDxfId="19"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="18"/>
-    <tableColumn id="3" name="[ifRule]" dataDxfId="17"/>
-    <tableColumn id="4" name="[thenTreeRule]" dataDxfId="16"/>
-    <tableColumn id="5" name="[elseTreeRule]" dataDxfId="15"/>
-    <tableColumn id="6" name="[thenResult]" dataDxfId="14"/>
-    <tableColumn id="7" name="[elseResult]" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{clusterRuleTreeDefinitions}" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[ifRule]" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[thenTreeRule]" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="[elseTreeRule]" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[thenResult]" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="[elseResult]" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings4" displayName="gameSettings4" ref="B64:D75" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
-  <autoFilter ref="B64:D75"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="gameSettings4" displayName="gameSettings4" ref="B64:D75" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+  <autoFilter ref="B64:D75" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{clusterRuleDefinitions}" dataDxfId="8"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="7"/>
-    <tableColumn id="3" name="[rule]" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="{clusterRuleDefinitions}" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="[sku]" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="[rule]" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="gameSettings45" displayName="gameSettings45" ref="B6:C10" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
-  <autoFilter ref="B6:C10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="gameSettings45" displayName="gameSettings45" ref="B6:C10" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
+  <autoFilter ref="B6:C10" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="{clusterDefinitions}" dataDxfId="1"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="{clusterDefinitions}" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="[sku]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1612,30 +1605,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
   <dimension ref="A3:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F87" sqref="F87"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="35.85546875" customWidth="1"/>
-    <col min="3" max="3" width="39.140625" customWidth="1"/>
-    <col min="4" max="4" width="97.140625" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="35.83203125" customWidth="1"/>
+    <col min="3" max="3" width="39.1640625" customWidth="1"/>
+    <col min="4" max="4" width="97.1640625" customWidth="1"/>
     <col min="5" max="5" width="27" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" customWidth="1"/>
     <col min="8" max="22" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:11" ht="24" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>16</v>
       </c>
@@ -1649,7 +1642,7 @@
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="8"/>
       <c r="B5" s="11"/>
       <c r="C5" s="9" t="s">
@@ -1664,7 +1657,7 @@
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="6" spans="1:11" ht="100.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="97" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
         <v>17</v>
       </c>
@@ -1672,7 +1665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>0</v>
       </c>
@@ -1680,36 +1673,36 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B11" s="13"/>
+      <c r="C11" s="14"/>
+    </row>
+    <row r="12" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:11" ht="24" x14ac:dyDescent="0.3">
       <c r="B13" s="7" t="s">
         <v>2</v>
       </c>
@@ -1723,7 +1716,7 @@
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="11"/>
       <c r="C14" s="9" t="s">
@@ -1738,7 +1731,7 @@
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="1:11" ht="119.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="115" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
         <v>3</v>
       </c>
@@ -1749,7 +1742,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
         <v>0</v>
       </c>
@@ -1760,8 +1753,10 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="C17" s="2" t="s">
         <v>56</v>
       </c>
@@ -1769,8 +1764,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="12"/>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="C18" s="2" t="s">
         <v>58</v>
       </c>
@@ -1778,8 +1775,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:11" ht="24" x14ac:dyDescent="0.3">
       <c r="B21" s="7" t="s">
         <v>10</v>
       </c>
@@ -1793,7 +1790,7 @@
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" ht="16" x14ac:dyDescent="0.2">
       <c r="B22" s="11"/>
       <c r="C22" s="10" t="s">
         <v>12</v>
@@ -1806,7 +1803,7 @@
       <c r="I22" s="9"/>
       <c r="J22" s="8"/>
     </row>
-    <row r="23" spans="2:11" ht="138.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" ht="134" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
         <v>7</v>
       </c>
@@ -1829,75 +1826,75 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24" s="21" t="s">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B24" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="17" t="s">
+      <c r="E24" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F24" s="17" t="s">
+      <c r="F24" s="16" t="s">
         <v>33</v>
       </c>
       <c r="G24" s="1"/>
-      <c r="H24" s="18"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" s="21" t="s">
+      <c r="H24" s="17"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B25" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="20" t="s">
         <v>32</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17" t="s">
+      <c r="E25" s="16"/>
+      <c r="F25" s="16" t="s">
         <v>34</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H25" s="13"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C26" s="21" t="s">
+      <c r="H25" s="12"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B26" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E26" s="17" t="s">
+      <c r="E26" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17" t="s">
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" s="21" t="s">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B27" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="20" t="s">
         <v>34</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
       <c r="G27" s="1" t="s">
         <v>20</v>
       </c>
@@ -1905,208 +1902,208 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" s="21" t="s">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B28" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17" t="s">
+      <c r="E28" s="16"/>
+      <c r="F28" s="16" t="s">
         <v>36</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H28" s="17"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" s="23" t="s">
+      <c r="H28" s="16"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B29" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="22" t="s">
         <v>36</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17" t="s">
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="H29" s="17" t="s">
+      <c r="H29" s="16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="26" t="s">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B30" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E30" s="13" t="s">
+      <c r="E30" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="F30" s="13" t="s">
+      <c r="F30" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" s="26" t="s">
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B31" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E31" s="27"/>
-      <c r="F31" s="13" t="s">
+      <c r="E31" s="26"/>
+      <c r="F31" s="12" t="s">
         <v>41</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H31" s="13"/>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B32" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="26" t="s">
+      <c r="H31" s="12"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B32" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E32" s="13" t="s">
+      <c r="E32" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="F32" s="13" t="s">
+      <c r="F32" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" s="26" t="s">
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B33" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="D33" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E33" s="27"/>
-      <c r="F33" s="13" t="s">
+      <c r="E33" s="26"/>
+      <c r="F33" s="12" t="s">
         <v>38</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H33" s="13"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C34" s="26" t="s">
+      <c r="H33" s="12"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B34" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="D34" s="13" t="s">
+      <c r="D34" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
       <c r="G34" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H34" s="17" t="s">
+      <c r="H34" s="16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C35" s="26" t="s">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B35" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="D35" s="13" t="s">
+      <c r="D35" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="E35" s="27"/>
-      <c r="F35" s="13" t="s">
+      <c r="E35" s="26"/>
+      <c r="F35" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="G35" s="17" t="s">
+      <c r="G35" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="H35" s="13"/>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C36" s="26" t="s">
+      <c r="H35" s="12"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B36" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="13" t="s">
+      <c r="D36" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E36" s="13" t="s">
+      <c r="E36" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F36" s="27"/>
-      <c r="G36" s="13"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="12"/>
       <c r="H36" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C37" s="26" t="s">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B37" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D37" s="13" t="s">
+      <c r="D37" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="E37" s="27"/>
-      <c r="F37" s="13" t="s">
+      <c r="E37" s="26"/>
+      <c r="F37" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="G37" s="17" t="s">
+      <c r="G37" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="H37" s="13"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C38" s="26" t="s">
+      <c r="H37" s="12"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B38" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="D38" s="13" t="s">
+      <c r="D38" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
       <c r="G38" s="1" t="s">
         <v>20</v>
       </c>
@@ -2114,105 +2111,113 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C39" s="26" t="s">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B39" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="D39" s="13" t="s">
+      <c r="D39" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="E39" s="27"/>
-      <c r="F39" s="13" t="s">
+      <c r="E39" s="26"/>
+      <c r="F39" s="12" t="s">
         <v>55</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H39" s="13"/>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C40" s="26" t="s">
+      <c r="H39" s="12"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B40" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="D40" s="17" t="s">
+      <c r="D40" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="17" t="s">
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="H40" s="17" t="s">
+      <c r="H40" s="16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="20"/>
-      <c r="C41" s="29" t="s">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B41" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="D41" s="17" t="s">
+      <c r="D41" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="E41" s="17" t="s">
+      <c r="E41" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="F41" s="17" t="s">
+      <c r="F41" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17"/>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="20"/>
-      <c r="C42" s="30" t="s">
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B42" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="D42" s="17" t="s">
+      <c r="D42" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="E42" s="17"/>
-      <c r="F42" s="17" t="s">
+      <c r="E42" s="16"/>
+      <c r="F42" s="16" t="s">
         <v>62</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H42" s="17"/>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="20"/>
-      <c r="C43" s="30" t="s">
+      <c r="H42" s="16"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B43" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="D43" s="17" t="s">
+      <c r="D43" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E43" s="17" t="s">
+      <c r="E43" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="F43" s="17" t="s">
+      <c r="F43" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="G43" s="17"/>
-      <c r="H43" s="17"/>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="20"/>
-      <c r="C44" s="30" t="s">
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B44" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="D44" s="17" t="s">
+      <c r="D44" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="E44" s="17"/>
-      <c r="F44" s="17"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
       <c r="G44" s="1" t="s">
         <v>20</v>
       </c>
@@ -2220,101 +2225,113 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="20"/>
-      <c r="C45" s="30" t="s">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B45" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="D45" s="17" t="s">
+      <c r="D45" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="E45" s="17" t="s">
+      <c r="E45" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="F45" s="17"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="17" t="s">
+      <c r="F45" s="16"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="20"/>
-      <c r="C46" s="30" t="s">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B46" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="D46" s="17" t="s">
+      <c r="D46" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="E46" s="17" t="s">
+      <c r="E46" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="F46" s="17" t="s">
+      <c r="F46" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="G46" s="13"/>
-      <c r="H46" s="13"/>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="20"/>
-      <c r="C47" s="30" t="s">
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B47" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="D47" s="17" t="s">
+      <c r="D47" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="E47" s="17"/>
-      <c r="F47" s="17"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
       <c r="G47" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H47" s="17" t="s">
+      <c r="H47" s="16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B48" s="20"/>
-      <c r="C48" s="30" t="s">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B48" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="D48" s="17" t="s">
+      <c r="D48" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E48" s="17" t="s">
+      <c r="E48" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="F48" s="17" t="s">
+      <c r="F48" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="G48" s="13"/>
-      <c r="H48" s="13"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B49" s="20"/>
-      <c r="C49" s="30" t="s">
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B49" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="D49" s="17" t="s">
+      <c r="D49" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E49" s="17"/>
-      <c r="F49" s="17" t="s">
+      <c r="E49" s="16"/>
+      <c r="F49" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="G49" s="17" t="s">
+      <c r="G49" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="H49" s="13"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B50" s="20"/>
-      <c r="C50" s="30" t="s">
+      <c r="H49" s="12"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B50" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="D50" s="17" t="s">
+      <c r="D50" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E50" s="17"/>
-      <c r="F50" s="17"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
       <c r="G50" s="1" t="s">
         <v>20</v>
       </c>
@@ -2322,161 +2339,179 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B51" s="20"/>
-      <c r="C51" s="30" t="s">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B51" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="D51" s="17" t="s">
+      <c r="D51" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="E51" s="17" t="s">
+      <c r="E51" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="F51" s="17" t="s">
+      <c r="F51" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="G51" s="17"/>
-      <c r="H51" s="17"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B52" s="20"/>
-      <c r="C52" s="30" t="s">
+      <c r="G51" s="16"/>
+      <c r="H51" s="16"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B52" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="D52" s="17" t="s">
+      <c r="D52" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="E52" s="17" t="s">
+      <c r="E52" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="F52" s="17" t="s">
+      <c r="F52" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="G52" s="17"/>
-      <c r="H52" s="17"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B53" s="20"/>
-      <c r="C53" s="30" t="s">
+      <c r="G52" s="16"/>
+      <c r="H52" s="16"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B53" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="D53" s="17" t="s">
+      <c r="D53" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="E53" s="17"/>
-      <c r="F53" s="17" t="s">
+      <c r="E53" s="16"/>
+      <c r="F53" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="G53" s="17" t="s">
+      <c r="G53" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="H53" s="17"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B54" s="20"/>
-      <c r="C54" s="30" t="s">
+      <c r="H53" s="16"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B54" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="D54" s="17" t="s">
+      <c r="D54" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="E54" s="17"/>
-      <c r="F54" s="17"/>
+      <c r="E54" s="16"/>
+      <c r="F54" s="16"/>
       <c r="G54" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H54" s="17" t="s">
+      <c r="H54" s="16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B55" s="20"/>
-      <c r="C55" s="30" t="s">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B55" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C55" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="D55" s="17" t="s">
+      <c r="D55" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="E55" s="17"/>
-      <c r="F55" s="17"/>
-      <c r="G55" s="17" t="s">
+      <c r="E55" s="16"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="H55" s="17" t="s">
+      <c r="H55" s="16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B56" s="20"/>
-      <c r="C56" s="30" t="s">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B56" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C56" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="D56" s="17" t="s">
+      <c r="D56" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="E56" s="17"/>
-      <c r="F56" s="17" t="s">
+      <c r="E56" s="16"/>
+      <c r="F56" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="G56" s="17" t="s">
+      <c r="G56" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="H56" s="17"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B57" s="20"/>
-      <c r="C57" s="30" t="s">
+      <c r="H56" s="16"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B57" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="D57" s="17" t="s">
+      <c r="D57" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="E57" s="17"/>
-      <c r="F57" s="17"/>
-      <c r="G57" s="17" t="s">
+      <c r="E57" s="16"/>
+      <c r="F57" s="16"/>
+      <c r="G57" s="16" t="s">
         <v>24</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B58" s="20"/>
-      <c r="C58" s="30" t="s">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B58" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C58" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="D58" s="17" t="s">
+      <c r="D58" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="E58" s="17" t="s">
+      <c r="E58" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="F58" s="17"/>
-      <c r="G58" s="13"/>
-      <c r="H58" s="17" t="s">
+      <c r="F58" s="16"/>
+      <c r="G58" s="12"/>
+      <c r="H58" s="16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B59" s="20"/>
-      <c r="C59" s="30" t="s">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B59" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="D59" s="17" t="s">
+      <c r="D59" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="E59" s="17"/>
-      <c r="F59" s="17"/>
-      <c r="G59" s="17" t="s">
+      <c r="E59" s="16"/>
+      <c r="F59" s="16"/>
+      <c r="G59" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="H59" s="17" t="s">
+      <c r="H59" s="16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="62" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:11" ht="24" x14ac:dyDescent="0.3">
       <c r="B62" s="7" t="s">
         <v>11</v>
       </c>
@@ -2490,7 +2525,7 @@
       <c r="J62" s="7"/>
       <c r="K62" s="7"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="8"/>
       <c r="B63" s="11"/>
       <c r="C63" s="9" t="s">
@@ -2505,7 +2540,7 @@
       <c r="J63" s="8"/>
       <c r="K63" s="8"/>
     </row>
-    <row r="64" spans="1:11" ht="119.25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" ht="115" x14ac:dyDescent="0.2">
       <c r="B64" s="6" t="s">
         <v>13</v>
       </c>
@@ -2516,359 +2551,416 @@
         <v>14</v>
       </c>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C65" s="24" t="s">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B65" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65" s="23" t="s">
         <v>31</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B66" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C66" s="24" t="s">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B66" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C66" s="23" t="s">
         <v>32</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C67" s="24" t="s">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B67" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C67" s="23" t="s">
         <v>33</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C68" s="24" t="s">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B68" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C68" s="23" t="s">
         <v>34</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B69" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C69" s="24" t="s">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B69" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C69" s="23" t="s">
         <v>35</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B70" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C70" s="24" t="s">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B70" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C70" s="23" t="s">
         <v>36</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C71" s="26" t="s">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B71" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C71" s="25" t="s">
         <v>37</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B72" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C72" s="26" t="s">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B72" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C72" s="25" t="s">
         <v>39</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C73" s="26" t="s">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B73" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C73" s="25" t="s">
         <v>40</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B74" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C74" s="26" t="s">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B74" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C74" s="25" t="s">
         <v>41</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C75" s="26" t="s">
+    <row r="75" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B75" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C75" s="25" t="s">
         <v>42</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B76" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C76" s="26" t="s">
+    <row r="76" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B76" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C76" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="D76" s="13" t="s">
+      <c r="D76" s="12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B77" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C77" s="26" t="s">
+    <row r="77" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B77" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C77" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="D77" s="13" t="s">
+      <c r="D77" s="12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B78" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C78" s="26" t="s">
+    <row r="78" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B78" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C78" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D78" s="13" t="s">
+      <c r="D78" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B79" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C79" s="26" t="s">
+    <row r="79" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B79" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C79" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="D79" s="13" t="s">
+      <c r="D79" s="12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B80" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C80" s="26" t="s">
+    <row r="80" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B80" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C80" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="D80" s="27" t="s">
+      <c r="D80" s="26" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B81" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C81" s="26" t="s">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B81" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C81" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="D81" s="27" t="s">
+      <c r="D81" s="26" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C82" s="31" t="s">
+    <row r="82" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B82" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C82" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="D82" s="13" t="s">
+      <c r="D82" s="12" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C83" s="31" t="s">
+    <row r="83" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B83" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C83" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="D83" s="13" t="s">
+      <c r="D83" s="12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C84" s="31" t="s">
+    <row r="84" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B84" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C84" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="D84" s="13" t="s">
+      <c r="D84" s="12" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C85" s="31" t="s">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B85" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C85" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="D85" s="13" t="s">
+      <c r="D85" s="12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C86" s="28" t="s">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B86" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C86" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="D86" s="13" t="s">
+      <c r="D86" s="12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C87" s="28" t="s">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B87" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C87" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="D87" s="13" t="s">
+      <c r="D87" s="12" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C88" s="28" t="s">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B88" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C88" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="D88" s="13" t="s">
+      <c r="D88" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F88" s="32"/>
-    </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C89" s="28" t="s">
+      <c r="F88" s="31"/>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B89" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C89" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="D89" s="13" t="s">
+      <c r="D89" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="F89" s="32"/>
-    </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C90" s="28" t="s">
+      <c r="F89" s="31"/>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B90" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C90" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="D90" s="27" t="s">
+      <c r="D90" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="F90" s="33"/>
-    </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C91" s="28" t="s">
+      <c r="F90" s="32"/>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B91" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C91" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="D91" s="13" t="s">
+      <c r="D91" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="F91" s="34"/>
-    </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C92" s="28" t="s">
+      <c r="F91" s="33"/>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B92" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C92" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="D92" s="27" t="s">
+      <c r="D92" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="F92" s="34"/>
-    </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C93" s="28" t="s">
+      <c r="F92" s="33"/>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B93" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C93" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="D93" s="27" t="s">
+      <c r="D93" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="F93" s="34"/>
-    </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C94" s="28" t="s">
+      <c r="F93" s="33"/>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B94" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C94" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="D94" s="27" t="s">
+      <c r="D94" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="F94" s="34"/>
-    </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C95" s="28" t="s">
+      <c r="F94" s="33"/>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B95" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C95" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="D95" s="27" t="s">
+      <c r="D95" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="F95" s="32"/>
-    </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C96" s="28" t="s">
+      <c r="F95" s="31"/>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B96" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C96" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="D96" s="13" t="s">
+      <c r="D96" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="F96" s="32"/>
-    </row>
-    <row r="97" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C97" s="28" t="s">
+      <c r="F96" s="31"/>
+    </row>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B97" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C97" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="D97" s="27" t="s">
+      <c r="D97" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="F97" s="32"/>
-    </row>
-    <row r="98" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C98" s="28" t="s">
+      <c r="F97" s="31"/>
+    </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B98" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C98" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="D98" s="13" t="s">
+      <c r="D98" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="F98" s="32"/>
-    </row>
-    <row r="99" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C99" s="28" t="s">
+      <c r="F98" s="31"/>
+    </row>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B99" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C99" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="D99" s="13" t="s">
+      <c r="D99" s="12" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="100" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C100" s="28" t="s">
+    <row r="100" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B100" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C100" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="D100" s="27" t="s">
+      <c r="D100" s="26" t="s">
         <v>90</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D79 D71 D65:E65 D7:E7 E25 E17:E18 D82 D86:D87 D96 D98:D99"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D79 D71 D65:E65 D7:E7 E25 E17:E18 D82 D86:D87 D96 D98:D99" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[FIX] Changed model for modelGroup
Former-commit-id: fa7ac6fae94d1b3a6489cf2067476e5218d5879d
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Clustering.xlsx
+++ b/Docs/Content/HungryDragonContent_Clustering.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mamuela/Repository/dragon/server/tools/scripts/clusterTreeValidator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mamuela/Repository/dragon/client/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240A0E4E-D962-F94C-9266-323FE995E900}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{95B811A7-6E27-004A-A13D-625E637C4DC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -300,13 +300,13 @@
     <t>model.boostTime &lt; 36e+3</t>
   </si>
   <si>
-    <t>["Huawei","ipad","iphone","Lenovo","Lge","Motorola","Oppo","Samsung"].indexOf(model.model) &gt;= 0</t>
-  </si>
-  <si>
-    <t>["ipad","Oppo","Samsung"].indexOf(model.model) &gt;= 0</t>
-  </si>
-  <si>
-    <t>["ipad","Lenovo","Lge","Motorola","Vivo","Samsung","Xiaomi"].indexOf(model.model) &gt;= 0</t>
+    <t>["Huawei","ipad","iphone","Lenovo","Lge","Motorola","Oppo","Samsung"].indexOf(model.modelGroup) &gt;= 0</t>
+  </si>
+  <si>
+    <t>["ipad","Oppo","Samsung"].indexOf(model.modelGroup) &gt;= 0</t>
+  </si>
+  <si>
+    <t>["ipad","Lenovo","Lge","Motorola","Vivo","Samsung","Xiaomi"].indexOf(model.modelGroup) &gt;= 0</t>
   </si>
 </sst>
 </file>
@@ -1612,7 +1612,7 @@
   <dimension ref="A3:K100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D93" sqref="D93"/>
+      <selection activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
[FIX] Fixed duplicated skus in content
Former-commit-id: b53e5fadbce237d94f87958114fcc9f3a3cf5d6e
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Clustering.xlsx
+++ b/Docs/Content/HungryDragonContent_Clustering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mamuela/Repository/dragon/client/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{95B811A7-6E27-004A-A13D-625E637C4DC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B5D902C-3BF2-DC41-A6DA-C233735B6E4D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="130">
   <si>
     <t>&lt;Definition&gt;</t>
   </si>
@@ -307,6 +307,114 @@
   </si>
   <si>
     <t>["ipad","Lenovo","Lge","Motorola","Vivo","Samsung","Xiaomi"].indexOf(model.modelGroup) &gt;= 0</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_001_NODE_001</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_001_NODE_002</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_001_NODE_003</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_001_NODE_004</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_001_NODE_005</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_001_NODE_006</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_002_NODE_001</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_002_NODE_002</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_002_NODE_003</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_002_NODE_004</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_002_NODE_005</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_002_NODE_006</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_002_NODE_007</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_002_NODE_008</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_002_NODE_009</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_002_NODE_010</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_002_NODE_011</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_003_NODE_001</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_003_NODE_002</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_003_NODE_003</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_003_NODE_004</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_003_NODE_005</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_003_NODE_006</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_003_NODE_007</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_003_NODE_008</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_003_NODE_009</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_003_NODE_010</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_003_NODE_011</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_003_NODE_012</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_003_NODE_013</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_003_NODE_014</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_003_NODE_015</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_003_NODE_016</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_003_NODE_017</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_003_NODE_018</t>
+  </si>
+  <si>
+    <t>CLUSTER_TREE_003_NODE_019</t>
   </si>
 </sst>
 </file>
@@ -514,7 +622,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -549,7 +657,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1611,8 +1718,8 @@
   </sheetPr>
   <dimension ref="A3:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E95" sqref="E95"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1750,7 +1857,7 @@
         <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>31</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
@@ -1761,7 +1868,7 @@
         <v>56</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>37</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
@@ -1772,7 +1879,7 @@
         <v>58</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>59</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -1831,16 +1938,16 @@
         <v>0</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>31</v>
+        <v>94</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>32</v>
+        <v>95</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="17"/>
@@ -1850,14 +1957,14 @@
         <v>0</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>32</v>
+        <v>95</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E25" s="16"/>
       <c r="F25" s="16" t="s">
-        <v>34</v>
+        <v>97</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>20</v>
@@ -1869,13 +1976,13 @@
         <v>0</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>35</v>
+        <v>98</v>
       </c>
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
@@ -1888,7 +1995,7 @@
         <v>0</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>34</v>
+        <v>97</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>34</v>
@@ -1907,14 +2014,14 @@
         <v>0</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>35</v>
+        <v>98</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E28" s="16"/>
       <c r="F28" s="16" t="s">
-        <v>36</v>
+        <v>99</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>20</v>
@@ -1925,8 +2032,8 @@
       <c r="B29" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C29" s="22" t="s">
-        <v>36</v>
+      <c r="C29" s="20" t="s">
+        <v>99</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>36</v>
@@ -1941,37 +2048,37 @@
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B30" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="25" t="s">
-        <v>37</v>
+      <c r="B30" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="24" t="s">
+        <v>100</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>37</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>39</v>
+        <v>101</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="G30" s="12"/>
       <c r="H30" s="12"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B31" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" s="25" t="s">
-        <v>39</v>
+      <c r="B31" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="24" t="s">
+        <v>101</v>
       </c>
       <c r="D31" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E31" s="26"/>
+      <c r="E31" s="25"/>
       <c r="F31" s="12" t="s">
-        <v>41</v>
+        <v>103</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>20</v>
@@ -1979,37 +2086,37 @@
       <c r="H31" s="12"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B32" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="25" t="s">
-        <v>40</v>
+      <c r="B32" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>102</v>
       </c>
       <c r="D32" s="12" t="s">
         <v>40</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>42</v>
+        <v>104</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="G32" s="12"/>
       <c r="H32" s="12"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B33" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" s="25" t="s">
-        <v>41</v>
+      <c r="B33" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="24" t="s">
+        <v>103</v>
       </c>
       <c r="D33" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E33" s="26"/>
+      <c r="E33" s="25"/>
       <c r="F33" s="12" t="s">
-        <v>38</v>
+        <v>106</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>20</v>
@@ -2017,17 +2124,17 @@
       <c r="H33" s="12"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B34" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C34" s="25" t="s">
-        <v>42</v>
+      <c r="B34" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="24" t="s">
+        <v>104</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
       <c r="G34" s="1" t="s">
         <v>20</v>
       </c>
@@ -2036,18 +2143,18 @@
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B35" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C35" s="25" t="s">
-        <v>45</v>
+      <c r="B35" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="24" t="s">
+        <v>105</v>
       </c>
       <c r="D35" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="E35" s="26"/>
+      <c r="E35" s="25"/>
       <c r="F35" s="12" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
       <c r="G35" s="16" t="s">
         <v>24</v>
@@ -2055,37 +2162,37 @@
       <c r="H35" s="12"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B36" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C36" s="25" t="s">
-        <v>38</v>
+      <c r="B36" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="24" t="s">
+        <v>106</v>
       </c>
       <c r="D36" s="12" t="s">
         <v>38</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F36" s="26"/>
+        <v>108</v>
+      </c>
+      <c r="F36" s="25"/>
       <c r="G36" s="12"/>
       <c r="H36" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B37" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C37" s="25" t="s">
-        <v>46</v>
+      <c r="B37" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="24" t="s">
+        <v>107</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="E37" s="26"/>
+      <c r="E37" s="25"/>
       <c r="F37" s="12" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="G37" s="16" t="s">
         <v>24</v>
@@ -2093,17 +2200,17 @@
       <c r="H37" s="12"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B38" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C38" s="25" t="s">
-        <v>47</v>
+      <c r="B38" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="24" t="s">
+        <v>108</v>
       </c>
       <c r="D38" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="25"/>
       <c r="G38" s="1" t="s">
         <v>20</v>
       </c>
@@ -2112,18 +2219,18 @@
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B39" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C39" s="25" t="s">
-        <v>53</v>
+      <c r="B39" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="24" t="s">
+        <v>109</v>
       </c>
       <c r="D39" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="E39" s="26"/>
+      <c r="E39" s="25"/>
       <c r="F39" s="12" t="s">
-        <v>55</v>
+        <v>110</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>23</v>
@@ -2131,17 +2238,17 @@
       <c r="H39" s="12"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B40" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C40" s="25" t="s">
-        <v>55</v>
+      <c r="B40" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="24" t="s">
+        <v>110</v>
       </c>
       <c r="D40" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="E40" s="26"/>
-      <c r="F40" s="26"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="25"/>
       <c r="G40" s="16" t="s">
         <v>24</v>
       </c>
@@ -2150,37 +2257,37 @@
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B41" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C41" s="28" t="s">
-        <v>59</v>
+      <c r="B41" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="27" t="s">
+        <v>111</v>
       </c>
       <c r="D41" s="16" t="s">
         <v>59</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="F41" s="16" t="s">
-        <v>61</v>
+        <v>113</v>
       </c>
       <c r="G41" s="16"/>
       <c r="H41" s="16"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B42" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C42" s="29" t="s">
-        <v>60</v>
+      <c r="B42" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="27" t="s">
+        <v>112</v>
       </c>
       <c r="D42" s="16" t="s">
         <v>60</v>
       </c>
       <c r="E42" s="16"/>
       <c r="F42" s="16" t="s">
-        <v>62</v>
+        <v>114</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>20</v>
@@ -2188,30 +2295,30 @@
       <c r="H42" s="16"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B43" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C43" s="29" t="s">
-        <v>61</v>
+      <c r="B43" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" s="27" t="s">
+        <v>113</v>
       </c>
       <c r="D43" s="16" t="s">
         <v>61</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>63</v>
+        <v>115</v>
       </c>
       <c r="F43" s="16" t="s">
-        <v>64</v>
+        <v>116</v>
       </c>
       <c r="G43" s="16"/>
       <c r="H43" s="16"/>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B44" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C44" s="29" t="s">
-        <v>62</v>
+      <c r="B44" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="27" t="s">
+        <v>114</v>
       </c>
       <c r="D44" s="16" t="s">
         <v>62</v>
@@ -2226,17 +2333,17 @@
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B45" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C45" s="29" t="s">
-        <v>63</v>
+      <c r="B45" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="27" t="s">
+        <v>115</v>
       </c>
       <c r="D45" s="16" t="s">
         <v>63</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>65</v>
+        <v>117</v>
       </c>
       <c r="F45" s="16"/>
       <c r="G45" s="12"/>
@@ -2245,30 +2352,30 @@
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B46" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C46" s="29" t="s">
-        <v>64</v>
+      <c r="B46" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="27" t="s">
+        <v>116</v>
       </c>
       <c r="D46" s="16" t="s">
         <v>64</v>
       </c>
       <c r="E46" s="16" t="s">
-        <v>66</v>
+        <v>118</v>
       </c>
       <c r="F46" s="16" t="s">
-        <v>67</v>
+        <v>119</v>
       </c>
       <c r="G46" s="12"/>
       <c r="H46" s="12"/>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B47" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C47" s="29" t="s">
-        <v>65</v>
+      <c r="B47" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="27" t="s">
+        <v>117</v>
       </c>
       <c r="D47" s="16" t="s">
         <v>65</v>
@@ -2283,37 +2390,37 @@
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B48" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C48" s="29" t="s">
-        <v>66</v>
+      <c r="B48" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="27" t="s">
+        <v>118</v>
       </c>
       <c r="D48" s="16" t="s">
         <v>66</v>
       </c>
       <c r="E48" s="16" t="s">
-        <v>68</v>
+        <v>120</v>
       </c>
       <c r="F48" s="16" t="s">
-        <v>69</v>
+        <v>121</v>
       </c>
       <c r="G48" s="12"/>
       <c r="H48" s="12"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B49" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C49" s="29" t="s">
-        <v>67</v>
+      <c r="B49" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="27" t="s">
+        <v>119</v>
       </c>
       <c r="D49" s="16" t="s">
         <v>67</v>
       </c>
       <c r="E49" s="16"/>
       <c r="F49" s="16" t="s">
-        <v>70</v>
+        <v>122</v>
       </c>
       <c r="G49" s="16" t="s">
         <v>24</v>
@@ -2321,11 +2428,11 @@
       <c r="H49" s="12"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B50" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C50" s="29" t="s">
-        <v>68</v>
+      <c r="B50" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="27" t="s">
+        <v>120</v>
       </c>
       <c r="D50" s="16" t="s">
         <v>68</v>
@@ -2340,56 +2447,56 @@
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B51" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C51" s="29" t="s">
-        <v>69</v>
+      <c r="B51" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="27" t="s">
+        <v>121</v>
       </c>
       <c r="D51" s="16" t="s">
         <v>69</v>
       </c>
       <c r="E51" s="16" t="s">
-        <v>71</v>
+        <v>123</v>
       </c>
       <c r="F51" s="16" t="s">
-        <v>72</v>
+        <v>124</v>
       </c>
       <c r="G51" s="16"/>
       <c r="H51" s="16"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B52" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C52" s="29" t="s">
-        <v>70</v>
+      <c r="B52" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" s="27" t="s">
+        <v>122</v>
       </c>
       <c r="D52" s="16" t="s">
         <v>70</v>
       </c>
       <c r="E52" s="16" t="s">
-        <v>73</v>
+        <v>125</v>
       </c>
       <c r="F52" s="16" t="s">
-        <v>74</v>
+        <v>126</v>
       </c>
       <c r="G52" s="16"/>
       <c r="H52" s="16"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B53" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C53" s="29" t="s">
-        <v>71</v>
+      <c r="B53" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" s="27" t="s">
+        <v>123</v>
       </c>
       <c r="D53" s="16" t="s">
         <v>71</v>
       </c>
       <c r="E53" s="16"/>
       <c r="F53" s="16" t="s">
-        <v>75</v>
+        <v>127</v>
       </c>
       <c r="G53" s="16" t="s">
         <v>24</v>
@@ -2397,11 +2504,11 @@
       <c r="H53" s="16"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B54" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C54" s="29" t="s">
-        <v>72</v>
+      <c r="B54" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" s="27" t="s">
+        <v>124</v>
       </c>
       <c r="D54" s="16" t="s">
         <v>72</v>
@@ -2416,11 +2523,11 @@
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B55" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C55" s="29" t="s">
-        <v>73</v>
+      <c r="B55" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C55" s="27" t="s">
+        <v>125</v>
       </c>
       <c r="D55" s="16" t="s">
         <v>73</v>
@@ -2435,18 +2542,18 @@
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B56" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C56" s="29" t="s">
-        <v>74</v>
+      <c r="B56" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C56" s="27" t="s">
+        <v>126</v>
       </c>
       <c r="D56" s="16" t="s">
         <v>74</v>
       </c>
       <c r="E56" s="16"/>
       <c r="F56" s="16" t="s">
-        <v>76</v>
+        <v>128</v>
       </c>
       <c r="G56" s="16" t="s">
         <v>24</v>
@@ -2454,11 +2561,11 @@
       <c r="H56" s="16"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B57" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C57" s="29" t="s">
-        <v>75</v>
+      <c r="B57" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" s="27" t="s">
+        <v>127</v>
       </c>
       <c r="D57" s="16" t="s">
         <v>75</v>
@@ -2473,17 +2580,17 @@
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B58" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C58" s="29" t="s">
-        <v>76</v>
+      <c r="B58" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C58" s="27" t="s">
+        <v>128</v>
       </c>
       <c r="D58" s="16" t="s">
         <v>76</v>
       </c>
       <c r="E58" s="16" t="s">
-        <v>77</v>
+        <v>129</v>
       </c>
       <c r="F58" s="16"/>
       <c r="G58" s="12"/>
@@ -2492,11 +2599,11 @@
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B59" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C59" s="29" t="s">
-        <v>77</v>
+      <c r="B59" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="27" t="s">
+        <v>129</v>
       </c>
       <c r="D59" s="16" t="s">
         <v>77</v>
@@ -2555,7 +2662,7 @@
       <c r="B65" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C65" s="23" t="s">
+      <c r="C65" s="22" t="s">
         <v>31</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -2566,7 +2673,7 @@
       <c r="B66" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C66" s="23" t="s">
+      <c r="C66" s="22" t="s">
         <v>32</v>
       </c>
       <c r="D66" s="1" t="s">
@@ -2577,7 +2684,7 @@
       <c r="B67" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C67" s="23" t="s">
+      <c r="C67" s="22" t="s">
         <v>33</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -2588,7 +2695,7 @@
       <c r="B68" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C68" s="23" t="s">
+      <c r="C68" s="22" t="s">
         <v>34</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -2599,7 +2706,7 @@
       <c r="B69" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C69" s="23" t="s">
+      <c r="C69" s="22" t="s">
         <v>35</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -2610,7 +2717,7 @@
       <c r="B70" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C70" s="23" t="s">
+      <c r="C70" s="22" t="s">
         <v>36</v>
       </c>
       <c r="D70" s="1" t="s">
@@ -2618,10 +2725,10 @@
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B71" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C71" s="25" t="s">
+      <c r="B71" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C71" s="24" t="s">
         <v>37</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -2629,10 +2736,10 @@
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B72" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C72" s="25" t="s">
+      <c r="B72" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C72" s="24" t="s">
         <v>39</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -2640,10 +2747,10 @@
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B73" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C73" s="25" t="s">
+      <c r="B73" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C73" s="24" t="s">
         <v>40</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -2651,10 +2758,10 @@
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B74" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C74" s="25" t="s">
+      <c r="B74" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C74" s="24" t="s">
         <v>41</v>
       </c>
       <c r="D74" s="1" t="s">
@@ -2662,10 +2769,10 @@
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B75" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C75" s="25" t="s">
+      <c r="B75" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C75" s="24" t="s">
         <v>42</v>
       </c>
       <c r="D75" s="1" t="s">
@@ -2673,10 +2780,10 @@
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B76" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C76" s="25" t="s">
+      <c r="B76" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C76" s="24" t="s">
         <v>45</v>
       </c>
       <c r="D76" s="12" t="s">
@@ -2684,10 +2791,10 @@
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B77" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C77" s="25" t="s">
+      <c r="B77" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C77" s="24" t="s">
         <v>38</v>
       </c>
       <c r="D77" s="12" t="s">
@@ -2695,10 +2802,10 @@
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B78" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C78" s="25" t="s">
+      <c r="B78" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C78" s="24" t="s">
         <v>46</v>
       </c>
       <c r="D78" s="12" t="s">
@@ -2706,10 +2813,10 @@
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B79" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C79" s="25" t="s">
+      <c r="B79" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C79" s="24" t="s">
         <v>47</v>
       </c>
       <c r="D79" s="12" t="s">
@@ -2717,32 +2824,32 @@
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B80" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C80" s="25" t="s">
+      <c r="B80" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C80" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D80" s="26" t="s">
+      <c r="D80" s="25" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B81" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C81" s="25" t="s">
+      <c r="B81" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C81" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="D81" s="26" t="s">
+      <c r="D81" s="25" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B82" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C82" s="30" t="s">
+      <c r="B82" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C82" s="29" t="s">
         <v>59</v>
       </c>
       <c r="D82" s="12" t="s">
@@ -2750,10 +2857,10 @@
       </c>
     </row>
     <row r="83" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B83" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C83" s="30" t="s">
+      <c r="B83" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C83" s="29" t="s">
         <v>60</v>
       </c>
       <c r="D83" s="12" t="s">
@@ -2761,10 +2868,10 @@
       </c>
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B84" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C84" s="30" t="s">
+      <c r="B84" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C84" s="29" t="s">
         <v>61</v>
       </c>
       <c r="D84" s="12" t="s">
@@ -2772,10 +2879,10 @@
       </c>
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B85" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C85" s="30" t="s">
+      <c r="B85" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C85" s="29" t="s">
         <v>62</v>
       </c>
       <c r="D85" s="12" t="s">
@@ -2783,10 +2890,10 @@
       </c>
     </row>
     <row r="86" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B86" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C86" s="27" t="s">
+      <c r="B86" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C86" s="26" t="s">
         <v>63</v>
       </c>
       <c r="D86" s="12" t="s">
@@ -2794,10 +2901,10 @@
       </c>
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B87" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C87" s="27" t="s">
+      <c r="B87" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C87" s="26" t="s">
         <v>64</v>
       </c>
       <c r="D87" s="12" t="s">
@@ -2805,142 +2912,142 @@
       </c>
     </row>
     <row r="88" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B88" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C88" s="27" t="s">
+      <c r="B88" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C88" s="26" t="s">
         <v>65</v>
       </c>
       <c r="D88" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F88" s="31"/>
+      <c r="F88" s="30"/>
     </row>
     <row r="89" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B89" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C89" s="27" t="s">
+      <c r="B89" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C89" s="26" t="s">
         <v>66</v>
       </c>
       <c r="D89" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="F89" s="31"/>
+      <c r="F89" s="30"/>
     </row>
     <row r="90" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B90" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C90" s="27" t="s">
+      <c r="B90" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C90" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="D90" s="26" t="s">
+      <c r="D90" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="F90" s="32"/>
+      <c r="F90" s="31"/>
     </row>
     <row r="91" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B91" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C91" s="27" t="s">
+      <c r="B91" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C91" s="26" t="s">
         <v>68</v>
       </c>
       <c r="D91" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="F91" s="33"/>
+      <c r="F91" s="32"/>
     </row>
     <row r="92" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B92" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C92" s="27" t="s">
+      <c r="B92" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C92" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="D92" s="26" t="s">
+      <c r="D92" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="F92" s="33"/>
+      <c r="F92" s="32"/>
     </row>
     <row r="93" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B93" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C93" s="27" t="s">
+      <c r="B93" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C93" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="D93" s="26" t="s">
+      <c r="D93" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="F93" s="33"/>
+      <c r="F93" s="32"/>
     </row>
     <row r="94" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B94" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C94" s="27" t="s">
+      <c r="B94" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C94" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="D94" s="26" t="s">
+      <c r="D94" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="F94" s="33"/>
+      <c r="F94" s="32"/>
     </row>
     <row r="95" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B95" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C95" s="27" t="s">
+      <c r="B95" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C95" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="D95" s="26" t="s">
+      <c r="D95" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="F95" s="31"/>
+      <c r="F95" s="30"/>
     </row>
     <row r="96" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B96" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C96" s="27" t="s">
+      <c r="B96" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C96" s="26" t="s">
         <v>73</v>
       </c>
       <c r="D96" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="F96" s="31"/>
+      <c r="F96" s="30"/>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B97" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C97" s="27" t="s">
+      <c r="B97" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C97" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="D97" s="26" t="s">
+      <c r="D97" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="F97" s="31"/>
+      <c r="F97" s="30"/>
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B98" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C98" s="27" t="s">
+      <c r="B98" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C98" s="26" t="s">
         <v>75</v>
       </c>
       <c r="D98" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="F98" s="31"/>
+      <c r="F98" s="30"/>
     </row>
     <row r="99" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B99" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C99" s="27" t="s">
+      <c r="B99" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C99" s="26" t="s">
         <v>76</v>
       </c>
       <c r="D99" s="12" t="s">
@@ -2948,13 +3055,13 @@
       </c>
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B100" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C100" s="27" t="s">
+      <c r="B100" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C100" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="D100" s="26" t="s">
+      <c r="D100" s="25" t="s">
         <v>90</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[FIX] replaced doublequotes for single
Former-commit-id: 4481d8f9bc80b71c7dcc2600d04d6a34030ad9df
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Clustering.xlsx
+++ b/Docs/Content/HungryDragonContent_Clustering.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mamuela/Repository/dragon/client/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B5D902C-3BF2-DC41-A6DA-C233735B6E4D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B08DE7-AA1E-7645-9412-55F9EF9913AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cluster" sheetId="2" r:id="rId1"/>
@@ -114,12 +114,6 @@
     <t>model.deviceProfile != 4</t>
   </si>
   <si>
-    <t>["GROUP_5","GROUP_6","GROUP_7","Others","Tier 1","Tier 2","Tier 3"].indexOf(model.countryGroup) &gt;= 0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">["GROUP_2","GROUP_3","GROUP_4"].indexOf(model.countryGroup) &gt;=0 </t>
-  </si>
-  <si>
     <t>CLUSTER_TREE_001_RULE_001</t>
   </si>
   <si>
@@ -159,9 +153,6 @@
     <t>model.deviceProfile == 0</t>
   </si>
   <si>
-    <t xml:space="preserve">["GROUP_3","GROUP_4"].indexOf(model.countryGroup) &gt;=0 </t>
-  </si>
-  <si>
     <t>CLUSTER_TREE_002_RULE_006</t>
   </si>
   <si>
@@ -177,12 +168,6 @@
     <t>model.score &lt; 12e+3</t>
   </si>
   <si>
-    <t xml:space="preserve">["GROUP_1","GROUP_2"].indexOf(model.countryGroup) &gt;=0 </t>
-  </si>
-  <si>
-    <t>["GROUP_5","Others","Tier 2"].indexOf(model.countryGroup) &gt;= 0</t>
-  </si>
-  <si>
     <t>model.boostTime &gt;= 186e+3</t>
   </si>
   <si>
@@ -198,9 +183,6 @@
     <t>CLUSTER_TREE_002</t>
   </si>
   <si>
-    <t>model.platform == "ANDROID"</t>
-  </si>
-  <si>
     <t>CLUSTER_TREE_003</t>
   </si>
   <si>
@@ -261,18 +243,9 @@
     <t>CLUSTER_TREE_003_RULE_019</t>
   </si>
   <si>
-    <t>["GROUP_5","GROUP_6","GROUP_7","Others","Tier 2","Tier 3"].indexOf(model.countryGroup) &gt;= 0</t>
-  </si>
-  <si>
     <t>model.score &lt; 14e+3</t>
   </si>
   <si>
-    <t>["GROUP_2","GROUP_3","GROUP_4","Tier 1"].indexOf(model.countryGroup) &gt;= 0</t>
-  </si>
-  <si>
-    <t>["GROUP_3","GROUP_4","Tier 1"].indexOf(model.countryGroup) &gt;= 0</t>
-  </si>
-  <si>
     <t>model.deviceProfile == 0 || model.deviceProfile == 1 || model.deviceProfile == 2</t>
   </si>
   <si>
@@ -300,15 +273,6 @@
     <t>model.boostTime &lt; 36e+3</t>
   </si>
   <si>
-    <t>["Huawei","ipad","iphone","Lenovo","Lge","Motorola","Oppo","Samsung"].indexOf(model.modelGroup) &gt;= 0</t>
-  </si>
-  <si>
-    <t>["ipad","Oppo","Samsung"].indexOf(model.modelGroup) &gt;= 0</t>
-  </si>
-  <si>
-    <t>["ipad","Lenovo","Lge","Motorola","Vivo","Samsung","Xiaomi"].indexOf(model.modelGroup) &gt;= 0</t>
-  </si>
-  <si>
     <t>CLUSTER_TREE_001_NODE_001</t>
   </si>
   <si>
@@ -415,6 +379,42 @@
   </si>
   <si>
     <t>CLUSTER_TREE_003_NODE_019</t>
+  </si>
+  <si>
+    <t>['GROUP_5','GROUP_6','GROUP_7','Others','Tier 1','Tier 2','Tier 3'].indexOf(model.countryGroup) &gt;= 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['GROUP_2','GROUP_3','GROUP_4'].indexOf(model.countryGroup) &gt;=0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['GROUP_3','GROUP_4'].indexOf(model.countryGroup) &gt;=0 </t>
+  </si>
+  <si>
+    <t>model.platform == 'ANDROID'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['GROUP_1','GROUP_2'].indexOf(model.countryGroup) &gt;=0 </t>
+  </si>
+  <si>
+    <t>['GROUP_5','Others','Tier 2'].indexOf(model.countryGroup) &gt;= 0</t>
+  </si>
+  <si>
+    <t>['GROUP_5','GROUP_6','GROUP_7','Others','Tier 2','Tier 3'].indexOf(model.countryGroup) &gt;= 0</t>
+  </si>
+  <si>
+    <t>['GROUP_2','GROUP_3','GROUP_4','Tier 1'].indexOf(model.countryGroup) &gt;= 0</t>
+  </si>
+  <si>
+    <t>['GROUP_3','GROUP_4','Tier 1'].indexOf(model.countryGroup) &gt;= 0</t>
+  </si>
+  <si>
+    <t>['Huawei','ipad','iphone','Lenovo','Lge','Motorola','Oppo','Samsung'].indexOf(model.modelGroup) &gt;= 0</t>
+  </si>
+  <si>
+    <t>['ipad','Oppo','Samsung'].indexOf(model.modelGroup) &gt;= 0</t>
+  </si>
+  <si>
+    <t>['ipad','Lenovo','Lge','Motorola','Vivo','Samsung','Xiaomi'].indexOf(model.modelGroup) &gt;= 0</t>
   </si>
 </sst>
 </file>
@@ -1718,8 +1718,8 @@
   </sheetPr>
   <dimension ref="A3:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1857,7 +1857,7 @@
         <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
@@ -1865,10 +1865,10 @@
         <v>0</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
@@ -1876,10 +1876,10 @@
         <v>0</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -1938,16 +1938,16 @@
         <v>0</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="17"/>
@@ -1957,14 +1957,14 @@
         <v>0</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E25" s="16"/>
       <c r="F25" s="16" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>20</v>
@@ -1976,13 +1976,13 @@
         <v>0</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
@@ -1995,10 +1995,10 @@
         <v>0</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E27" s="16"/>
       <c r="F27" s="16"/>
@@ -2014,14 +2014,14 @@
         <v>0</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E28" s="16"/>
       <c r="F28" s="16" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>20</v>
@@ -2033,10 +2033,10 @@
         <v>0</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
@@ -2052,16 +2052,16 @@
         <v>0</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="G30" s="12"/>
       <c r="H30" s="12"/>
@@ -2071,14 +2071,14 @@
         <v>0</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E31" s="25"/>
       <c r="F31" s="12" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>20</v>
@@ -2090,16 +2090,16 @@
         <v>0</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="G32" s="12"/>
       <c r="H32" s="12"/>
@@ -2109,14 +2109,14 @@
         <v>0</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E33" s="25"/>
       <c r="F33" s="12" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>20</v>
@@ -2128,10 +2128,10 @@
         <v>0</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E34" s="25"/>
       <c r="F34" s="25"/>
@@ -2147,14 +2147,14 @@
         <v>0</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E35" s="25"/>
       <c r="F35" s="12" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="G35" s="16" t="s">
         <v>24</v>
@@ -2166,13 +2166,13 @@
         <v>0</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="F36" s="25"/>
       <c r="G36" s="12"/>
@@ -2185,14 +2185,14 @@
         <v>0</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E37" s="25"/>
       <c r="F37" s="12" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="G37" s="16" t="s">
         <v>24</v>
@@ -2204,10 +2204,10 @@
         <v>0</v>
       </c>
       <c r="C38" s="24" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E38" s="25"/>
       <c r="F38" s="25"/>
@@ -2223,14 +2223,14 @@
         <v>0</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E39" s="25"/>
       <c r="F39" s="12" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>23</v>
@@ -2242,10 +2242,10 @@
         <v>0</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E40" s="25"/>
       <c r="F40" s="25"/>
@@ -2261,16 +2261,16 @@
         <v>0</v>
       </c>
       <c r="C41" s="27" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F41" s="16" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="G41" s="16"/>
       <c r="H41" s="16"/>
@@ -2280,14 +2280,14 @@
         <v>0</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E42" s="16"/>
       <c r="F42" s="16" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>20</v>
@@ -2299,16 +2299,16 @@
         <v>0</v>
       </c>
       <c r="C43" s="27" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="F43" s="16" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="G43" s="16"/>
       <c r="H43" s="16"/>
@@ -2318,10 +2318,10 @@
         <v>0</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E44" s="16"/>
       <c r="F44" s="16"/>
@@ -2337,13 +2337,13 @@
         <v>0</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="F45" s="16"/>
       <c r="G45" s="12"/>
@@ -2356,16 +2356,16 @@
         <v>0</v>
       </c>
       <c r="C46" s="27" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E46" s="16" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="F46" s="16" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="G46" s="12"/>
       <c r="H46" s="12"/>
@@ -2375,10 +2375,10 @@
         <v>0</v>
       </c>
       <c r="C47" s="27" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E47" s="16"/>
       <c r="F47" s="16"/>
@@ -2394,16 +2394,16 @@
         <v>0</v>
       </c>
       <c r="C48" s="27" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E48" s="16" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="F48" s="16" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="G48" s="12"/>
       <c r="H48" s="12"/>
@@ -2413,14 +2413,14 @@
         <v>0</v>
       </c>
       <c r="C49" s="27" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E49" s="16"/>
       <c r="F49" s="16" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="G49" s="16" t="s">
         <v>24</v>
@@ -2432,10 +2432,10 @@
         <v>0</v>
       </c>
       <c r="C50" s="27" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E50" s="16"/>
       <c r="F50" s="16"/>
@@ -2451,16 +2451,16 @@
         <v>0</v>
       </c>
       <c r="C51" s="27" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E51" s="16" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="F51" s="16" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="G51" s="16"/>
       <c r="H51" s="16"/>
@@ -2470,16 +2470,16 @@
         <v>0</v>
       </c>
       <c r="C52" s="27" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E52" s="16" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F52" s="16" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="G52" s="16"/>
       <c r="H52" s="16"/>
@@ -2489,14 +2489,14 @@
         <v>0</v>
       </c>
       <c r="C53" s="27" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="D53" s="16" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E53" s="16"/>
       <c r="F53" s="16" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="G53" s="16" t="s">
         <v>24</v>
@@ -2508,10 +2508,10 @@
         <v>0</v>
       </c>
       <c r="C54" s="27" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E54" s="16"/>
       <c r="F54" s="16"/>
@@ -2527,10 +2527,10 @@
         <v>0</v>
       </c>
       <c r="C55" s="27" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="D55" s="16" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E55" s="16"/>
       <c r="F55" s="16"/>
@@ -2546,14 +2546,14 @@
         <v>0</v>
       </c>
       <c r="C56" s="27" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="D56" s="16" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E56" s="16"/>
       <c r="F56" s="16" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="G56" s="16" t="s">
         <v>24</v>
@@ -2565,10 +2565,10 @@
         <v>0</v>
       </c>
       <c r="C57" s="27" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="D57" s="16" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E57" s="16"/>
       <c r="F57" s="16"/>
@@ -2584,13 +2584,13 @@
         <v>0</v>
       </c>
       <c r="C58" s="27" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="D58" s="16" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E58" s="16" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="F58" s="16"/>
       <c r="G58" s="12"/>
@@ -2603,10 +2603,10 @@
         <v>0</v>
       </c>
       <c r="C59" s="27" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="D59" s="16" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E59" s="16"/>
       <c r="F59" s="16"/>
@@ -2663,10 +2663,10 @@
         <v>0</v>
       </c>
       <c r="C65" s="22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>29</v>
+        <v>118</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.2">
@@ -2674,7 +2674,7 @@
         <v>0</v>
       </c>
       <c r="C66" s="22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>26</v>
@@ -2685,10 +2685,10 @@
         <v>0</v>
       </c>
       <c r="C67" s="22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>30</v>
+        <v>119</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.2">
@@ -2696,7 +2696,7 @@
         <v>0</v>
       </c>
       <c r="C68" s="22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>27</v>
@@ -2707,7 +2707,7 @@
         <v>0</v>
       </c>
       <c r="C69" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>28</v>
@@ -2718,10 +2718,10 @@
         <v>0</v>
       </c>
       <c r="C70" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.2">
@@ -2729,10 +2729,10 @@
         <v>0</v>
       </c>
       <c r="C71" s="24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>29</v>
+        <v>118</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.2">
@@ -2740,10 +2740,10 @@
         <v>0</v>
       </c>
       <c r="C72" s="24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.2">
@@ -2751,7 +2751,7 @@
         <v>0</v>
       </c>
       <c r="C73" s="24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>28</v>
@@ -2762,10 +2762,10 @@
         <v>0</v>
       </c>
       <c r="C74" s="24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.2">
@@ -2773,10 +2773,10 @@
         <v>0</v>
       </c>
       <c r="C75" s="24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>44</v>
+        <v>120</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.2">
@@ -2784,10 +2784,10 @@
         <v>0</v>
       </c>
       <c r="C76" s="24" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D76" s="12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.2">
@@ -2795,10 +2795,10 @@
         <v>0</v>
       </c>
       <c r="C77" s="24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D77" s="12" t="s">
-        <v>57</v>
+        <v>121</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.2">
@@ -2806,10 +2806,10 @@
         <v>0</v>
       </c>
       <c r="C78" s="24" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D78" s="12" t="s">
-        <v>50</v>
+        <v>122</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.2">
@@ -2817,10 +2817,10 @@
         <v>0</v>
       </c>
       <c r="C79" s="24" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D79" s="12" t="s">
-        <v>51</v>
+        <v>123</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.2">
@@ -2828,10 +2828,10 @@
         <v>0</v>
       </c>
       <c r="C80" s="24" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D80" s="25" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.2">
@@ -2839,10 +2839,10 @@
         <v>0</v>
       </c>
       <c r="C81" s="24" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D81" s="25" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.2">
@@ -2850,10 +2850,10 @@
         <v>0</v>
       </c>
       <c r="C82" s="29" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D82" s="12" t="s">
-        <v>78</v>
+        <v>124</v>
       </c>
     </row>
     <row r="83" spans="2:6" x14ac:dyDescent="0.2">
@@ -2861,10 +2861,10 @@
         <v>0</v>
       </c>
       <c r="C83" s="29" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D83" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.2">
@@ -2872,10 +2872,10 @@
         <v>0</v>
       </c>
       <c r="C84" s="29" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D84" s="12" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.2">
@@ -2883,10 +2883,10 @@
         <v>0</v>
       </c>
       <c r="C85" s="29" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D85" s="12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="86" spans="2:6" x14ac:dyDescent="0.2">
@@ -2894,10 +2894,10 @@
         <v>0</v>
       </c>
       <c r="C86" s="26" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D86" s="12" t="s">
-        <v>80</v>
+        <v>125</v>
       </c>
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.2">
@@ -2905,10 +2905,10 @@
         <v>0</v>
       </c>
       <c r="C87" s="26" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D87" s="12" t="s">
-        <v>81</v>
+        <v>126</v>
       </c>
     </row>
     <row r="88" spans="2:6" x14ac:dyDescent="0.2">
@@ -2916,7 +2916,7 @@
         <v>0</v>
       </c>
       <c r="C88" s="26" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D88" s="12" t="s">
         <v>28</v>
@@ -2928,10 +2928,10 @@
         <v>0</v>
       </c>
       <c r="C89" s="26" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D89" s="12" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="F89" s="30"/>
     </row>
@@ -2940,10 +2940,10 @@
         <v>0</v>
       </c>
       <c r="C90" s="26" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D90" s="25" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="F90" s="31"/>
     </row>
@@ -2952,10 +2952,10 @@
         <v>0</v>
       </c>
       <c r="C91" s="26" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D91" s="12" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F91" s="32"/>
     </row>
@@ -2964,10 +2964,10 @@
         <v>0</v>
       </c>
       <c r="C92" s="26" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D92" s="25" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="F92" s="32"/>
     </row>
@@ -2976,10 +2976,10 @@
         <v>0</v>
       </c>
       <c r="C93" s="26" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D93" s="25" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="F93" s="32"/>
     </row>
@@ -2988,10 +2988,10 @@
         <v>0</v>
       </c>
       <c r="C94" s="26" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D94" s="25" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="F94" s="32"/>
     </row>
@@ -3000,10 +3000,10 @@
         <v>0</v>
       </c>
       <c r="C95" s="26" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D95" s="25" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="F95" s="30"/>
     </row>
@@ -3012,10 +3012,10 @@
         <v>0</v>
       </c>
       <c r="C96" s="26" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D96" s="12" t="s">
-        <v>91</v>
+        <v>127</v>
       </c>
       <c r="F96" s="30"/>
     </row>
@@ -3024,10 +3024,10 @@
         <v>0</v>
       </c>
       <c r="C97" s="26" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D97" s="25" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F97" s="30"/>
     </row>
@@ -3036,10 +3036,10 @@
         <v>0</v>
       </c>
       <c r="C98" s="26" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D98" s="12" t="s">
-        <v>92</v>
+        <v>128</v>
       </c>
       <c r="F98" s="30"/>
     </row>
@@ -3048,10 +3048,10 @@
         <v>0</v>
       </c>
       <c r="C99" s="26" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D99" s="12" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.2">
@@ -3059,10 +3059,10 @@
         <v>0</v>
       </c>
       <c r="C100" s="26" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D100" s="25" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX] Fixed tier names on excel
Former-commit-id: c5fc8d85ab6234b32771444a4971737beb6febc4
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Clustering.xlsx
+++ b/Docs/Content/HungryDragonContent_Clustering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mamuela/Repository/dragon/client/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B08DE7-AA1E-7645-9412-55F9EF9913AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{04F84A55-5CB6-1343-941D-517E8F88436F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -381,9 +381,6 @@
     <t>CLUSTER_TREE_003_NODE_019</t>
   </si>
   <si>
-    <t>['GROUP_5','GROUP_6','GROUP_7','Others','Tier 1','Tier 2','Tier 3'].indexOf(model.countryGroup) &gt;= 0</t>
-  </si>
-  <si>
     <t xml:space="preserve">['GROUP_2','GROUP_3','GROUP_4'].indexOf(model.countryGroup) &gt;=0 </t>
   </si>
   <si>
@@ -396,18 +393,6 @@
     <t xml:space="preserve">['GROUP_1','GROUP_2'].indexOf(model.countryGroup) &gt;=0 </t>
   </si>
   <si>
-    <t>['GROUP_5','Others','Tier 2'].indexOf(model.countryGroup) &gt;= 0</t>
-  </si>
-  <si>
-    <t>['GROUP_5','GROUP_6','GROUP_7','Others','Tier 2','Tier 3'].indexOf(model.countryGroup) &gt;= 0</t>
-  </si>
-  <si>
-    <t>['GROUP_2','GROUP_3','GROUP_4','Tier 1'].indexOf(model.countryGroup) &gt;= 0</t>
-  </si>
-  <si>
-    <t>['GROUP_3','GROUP_4','Tier 1'].indexOf(model.countryGroup) &gt;= 0</t>
-  </si>
-  <si>
     <t>['Huawei','ipad','iphone','Lenovo','Lge','Motorola','Oppo','Samsung'].indexOf(model.modelGroup) &gt;= 0</t>
   </si>
   <si>
@@ -415,6 +400,21 @@
   </si>
   <si>
     <t>['ipad','Lenovo','Lge','Motorola','Vivo','Samsung','Xiaomi'].indexOf(model.modelGroup) &gt;= 0</t>
+  </si>
+  <si>
+    <t>['GROUP_2','GROUP_3','GROUP_4','TIER_1'].indexOf(model.countryGroup) &gt;= 0</t>
+  </si>
+  <si>
+    <t>['GROUP_3','GROUP_4','TIER_1'].indexOf(model.countryGroup) &gt;= 0</t>
+  </si>
+  <si>
+    <t>['GROUP_5','GROUP_6','GROUP_7','OTHERS','TIER_1','TIER_2','TIER_3'].indexOf(model.countryGroup) &gt;= 0</t>
+  </si>
+  <si>
+    <t>['GROUP_5','OTHERS','TIER_2'].indexOf(model.countryGroup) &gt;= 0</t>
+  </si>
+  <si>
+    <t>['GROUP_5','GROUP_6','GROUP_7','OTHERS','TIER_2','TIER_3'].indexOf(model.countryGroup) &gt;= 0</t>
   </si>
 </sst>
 </file>
@@ -1718,8 +1718,8 @@
   </sheetPr>
   <dimension ref="A3:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2666,7 +2666,7 @@
         <v>29</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.2">
@@ -2688,7 +2688,7 @@
         <v>31</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.2">
@@ -2732,7 +2732,7 @@
         <v>35</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.2">
@@ -2776,7 +2776,7 @@
         <v>40</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.2">
@@ -2798,7 +2798,7 @@
         <v>36</v>
       </c>
       <c r="D77" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.2">
@@ -2809,7 +2809,7 @@
         <v>43</v>
       </c>
       <c r="D78" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.2">
@@ -2820,7 +2820,7 @@
         <v>44</v>
       </c>
       <c r="D79" s="12" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.2">
@@ -2853,7 +2853,7 @@
         <v>53</v>
       </c>
       <c r="D82" s="12" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="83" spans="2:6" x14ac:dyDescent="0.2">
@@ -3015,7 +3015,7 @@
         <v>67</v>
       </c>
       <c r="D96" s="12" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F96" s="30"/>
     </row>
@@ -3039,7 +3039,7 @@
         <v>69</v>
       </c>
       <c r="D98" s="12" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F98" s="30"/>
     </row>
@@ -3051,7 +3051,7 @@
         <v>70</v>
       </c>
       <c r="D99" s="12" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
New trees and XML
Former-commit-id: 00c90daab3cb2b2d2d15de0074e751011d0fcb3d
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Clustering.xlsx
+++ b/Docs/Content/HungryDragonContent_Clustering.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="147">
   <si>
     <t>&lt;Definition&gt;</t>
   </si>
@@ -471,7 +471,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -514,13 +514,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -701,7 +694,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -738,10 +731,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
@@ -751,383 +742,18 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="31">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1251,6 +877,99 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
         <top style="thin">
           <color auto="1"/>
@@ -1302,6 +1021,282 @@
           <color auto="1"/>
         </right>
         <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
         <bottom/>
       </border>
     </dxf>
@@ -1545,36 +1540,36 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B23:H66" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
   <autoFilter ref="B23:H66"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{clusterRuleTreeDefinitions}" dataDxfId="6"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="5"/>
-    <tableColumn id="3" name="[ifRule]" dataDxfId="4"/>
-    <tableColumn id="4" name="[thenTreeRule]" dataDxfId="3"/>
-    <tableColumn id="5" name="[elseTreeRule]" dataDxfId="2"/>
-    <tableColumn id="6" name="[thenResult]" dataDxfId="1"/>
-    <tableColumn id="7" name="[elseResult]" dataDxfId="0"/>
+    <tableColumn id="1" name="{clusterRuleTreeDefinitions}" dataDxfId="19"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="18"/>
+    <tableColumn id="3" name="[ifRule]" dataDxfId="17"/>
+    <tableColumn id="4" name="[thenTreeRule]" dataDxfId="16"/>
+    <tableColumn id="5" name="[elseTreeRule]" dataDxfId="15"/>
+    <tableColumn id="6" name="[thenResult]" dataDxfId="14"/>
+    <tableColumn id="7" name="[elseResult]" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings4" displayName="gameSettings4" ref="B84:D127" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings4" displayName="gameSettings4" ref="B84:D127" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
   <autoFilter ref="B84:D127"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{clusterRuleDefinitions}" dataDxfId="9"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="8"/>
-    <tableColumn id="3" name="[rule]" dataDxfId="7"/>
+    <tableColumn id="1" name="{clusterRuleDefinitions}" dataDxfId="8"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="7"/>
+    <tableColumn id="3" name="[rule]" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="gameSettings45" displayName="gameSettings45" ref="B6:C10" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13" totalsRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="gameSettings45" displayName="gameSettings45" ref="B6:C10" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
   <autoFilter ref="B6:C10"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="{clusterDefinitions}" dataDxfId="11"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="10"/>
+    <tableColumn id="1" name="{clusterDefinitions}" dataDxfId="1"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1848,8 +1843,8 @@
   </sheetPr>
   <dimension ref="A3:K197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H60" sqref="H60"/>
+    <sheetView tabSelected="1" topLeftCell="D34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H66" sqref="H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2045,27 +2040,27 @@
       <c r="B23" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="29" t="s">
+      <c r="D23" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="29" t="s">
+      <c r="E23" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F23" s="29" t="s">
+      <c r="F23" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="G23" s="29" t="s">
+      <c r="G23" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="H23" s="29" t="s">
+      <c r="H23" s="27" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="30" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="22" t="s">
@@ -2084,7 +2079,7 @@
       <c r="H24" s="12"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="24" t="s">
         <v>0</v>
       </c>
       <c r="C25" s="22" t="s">
@@ -2103,7 +2098,7 @@
       <c r="H25" s="12"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="24" t="s">
         <v>0</v>
       </c>
       <c r="C26" s="22" t="s">
@@ -2122,7 +2117,7 @@
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="24" t="s">
         <v>0</v>
       </c>
       <c r="C27" s="22" t="s">
@@ -2141,7 +2136,7 @@
       <c r="H27" s="12"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="24" t="s">
         <v>0</v>
       </c>
       <c r="C28" s="22" t="s">
@@ -2160,7 +2155,7 @@
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="24" t="s">
         <v>0</v>
       </c>
       <c r="C29" s="22" t="s">
@@ -2179,7 +2174,7 @@
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="30" t="s">
         <v>0</v>
       </c>
       <c r="C30" s="22" t="s">
@@ -2198,7 +2193,7 @@
       <c r="H30" s="12"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="23" t="s">
+      <c r="B31" s="30" t="s">
         <v>0</v>
       </c>
       <c r="C31" s="22" t="s">
@@ -2217,7 +2212,7 @@
       <c r="H31" s="12"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B32" s="23" t="s">
+      <c r="B32" s="30" t="s">
         <v>0</v>
       </c>
       <c r="C32" s="22" t="s">
@@ -2236,7 +2231,7 @@
       <c r="H32" s="12"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="23" t="s">
+      <c r="B33" s="30" t="s">
         <v>0</v>
       </c>
       <c r="C33" s="22" t="s">
@@ -2255,7 +2250,7 @@
       <c r="H33" s="12"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="23" t="s">
+      <c r="B34" s="30" t="s">
         <v>0</v>
       </c>
       <c r="C34" s="22" t="s">
@@ -2274,7 +2269,7 @@
       <c r="H34" s="12"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="23" t="s">
+      <c r="B35" s="30" t="s">
         <v>0</v>
       </c>
       <c r="C35" s="22" t="s">
@@ -2293,7 +2288,7 @@
       <c r="H35" s="12"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="23" t="s">
+      <c r="B36" s="30" t="s">
         <v>0</v>
       </c>
       <c r="C36" s="22" t="s">
@@ -2312,7 +2307,7 @@
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="23" t="s">
+      <c r="B37" s="30" t="s">
         <v>0</v>
       </c>
       <c r="C37" s="22" t="s">
@@ -2331,7 +2326,7 @@
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="23" t="s">
+      <c r="B38" s="30" t="s">
         <v>0</v>
       </c>
       <c r="C38" s="22" t="s">
@@ -2350,7 +2345,7 @@
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="23" t="s">
+      <c r="B39" s="30" t="s">
         <v>0</v>
       </c>
       <c r="C39" s="22" t="s">
@@ -2369,7 +2364,7 @@
       <c r="H39" s="12"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="23" t="s">
+      <c r="B40" s="30" t="s">
         <v>0</v>
       </c>
       <c r="C40" s="22" t="s">
@@ -2388,7 +2383,7 @@
       <c r="H40" s="12"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="33" t="s">
+      <c r="B41" s="31" t="s">
         <v>0</v>
       </c>
       <c r="C41" s="22" t="s">
@@ -2407,7 +2402,7 @@
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="33" t="s">
+      <c r="B42" s="31" t="s">
         <v>0</v>
       </c>
       <c r="C42" s="22" t="s">
@@ -2426,7 +2421,7 @@
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="33" t="s">
+      <c r="B43" s="31" t="s">
         <v>0</v>
       </c>
       <c r="C43" s="22" t="s">
@@ -2445,10 +2440,10 @@
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C44" s="31" t="s">
+      <c r="B44" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="29" t="s">
         <v>65</v>
       </c>
       <c r="D44" s="12" t="s">
@@ -2464,10 +2459,10 @@
       <c r="H44" s="12"/>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C45" s="31" t="s">
+      <c r="B45" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="29" t="s">
         <v>66</v>
       </c>
       <c r="D45" s="12" t="s">
@@ -2483,10 +2478,10 @@
       <c r="H45" s="12"/>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C46" s="31" t="s">
+      <c r="B46" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="29" t="s">
         <v>67</v>
       </c>
       <c r="D46" s="12" t="s">
@@ -2502,10 +2497,10 @@
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C47" s="31" t="s">
+      <c r="B47" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="29" t="s">
         <v>68</v>
       </c>
       <c r="D47" s="12" t="s">
@@ -2521,10 +2516,10 @@
       <c r="H47" s="12"/>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B48" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C48" s="31" t="s">
+      <c r="B48" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="29" t="s">
         <v>69</v>
       </c>
       <c r="D48" s="12" t="s">
@@ -2540,10 +2535,10 @@
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C49" s="31" t="s">
+      <c r="B49" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="29" t="s">
         <v>70</v>
       </c>
       <c r="D49" s="12" t="s">
@@ -2559,10 +2554,10 @@
       <c r="H49" s="12"/>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C50" s="31" t="s">
+      <c r="B50" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="29" t="s">
         <v>71</v>
       </c>
       <c r="D50" s="12" t="s">
@@ -2578,10 +2573,10 @@
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B51" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C51" s="31" t="s">
+      <c r="B51" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="29" t="s">
         <v>72</v>
       </c>
       <c r="D51" s="12" t="s">
@@ -2597,10 +2592,10 @@
       <c r="H51" s="12"/>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B52" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C52" s="31" t="s">
+      <c r="B52" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" s="29" t="s">
         <v>73</v>
       </c>
       <c r="D52" s="12" t="s">
@@ -2616,10 +2611,10 @@
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B53" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C53" s="31" t="s">
+      <c r="B53" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" s="29" t="s">
         <v>74</v>
       </c>
       <c r="D53" s="12" t="s">
@@ -2635,10 +2630,10 @@
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B54" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C54" s="31" t="s">
+      <c r="B54" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" s="29" t="s">
         <v>75</v>
       </c>
       <c r="D54" s="12" t="s">
@@ -2654,7 +2649,7 @@
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B55" s="33" t="s">
+      <c r="B55" s="34" t="s">
         <v>0</v>
       </c>
       <c r="C55" s="18" t="s">
@@ -2673,7 +2668,7 @@
       <c r="H55" s="12"/>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B56" s="33" t="s">
+      <c r="B56" s="35" t="s">
         <v>0</v>
       </c>
       <c r="C56" s="18" t="s">
@@ -2692,7 +2687,7 @@
       <c r="H56" s="12"/>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B57" s="33" t="s">
+      <c r="B57" s="35" t="s">
         <v>0</v>
       </c>
       <c r="C57" s="18" t="s">
@@ -2711,7 +2706,7 @@
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B58" s="33" t="s">
+      <c r="B58" s="35" t="s">
         <v>0</v>
       </c>
       <c r="C58" s="18" t="s">
@@ -2730,7 +2725,7 @@
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B59" s="33" t="s">
+      <c r="B59" s="35" t="s">
         <v>0</v>
       </c>
       <c r="C59" s="18" t="s">
@@ -2749,7 +2744,9 @@
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B60" s="35"/>
+      <c r="B60" s="35" t="s">
+        <v>0</v>
+      </c>
       <c r="C60" s="18" t="s">
         <v>81</v>
       </c>
@@ -2766,7 +2763,9 @@
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B61" s="35"/>
+      <c r="B61" s="35" t="s">
+        <v>0</v>
+      </c>
       <c r="C61" s="18" t="s">
         <v>82</v>
       </c>
@@ -2783,7 +2782,9 @@
       <c r="H61" s="12"/>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B62" s="35"/>
+      <c r="B62" s="35" t="s">
+        <v>0</v>
+      </c>
       <c r="C62" s="18" t="s">
         <v>83</v>
       </c>
@@ -2800,7 +2801,9 @@
       <c r="H62" s="12"/>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B63" s="35"/>
+      <c r="B63" s="35" t="s">
+        <v>0</v>
+      </c>
       <c r="C63" s="18" t="s">
         <v>84</v>
       </c>
@@ -2817,7 +2820,9 @@
       <c r="H63" s="12"/>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B64" s="35"/>
+      <c r="B64" s="35" t="s">
+        <v>0</v>
+      </c>
       <c r="C64" s="18" t="s">
         <v>85</v>
       </c>
@@ -2834,7 +2839,9 @@
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B65" s="35"/>
+      <c r="B65" s="35" t="s">
+        <v>0</v>
+      </c>
       <c r="C65" s="18" t="s">
         <v>86</v>
       </c>
@@ -2851,7 +2858,9 @@
       <c r="H65" s="12"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B66" s="35"/>
+      <c r="B66" s="36" t="s">
+        <v>0</v>
+      </c>
       <c r="C66" s="18" t="s">
         <v>87</v>
       </c>
@@ -2868,9 +2877,7 @@
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B67" s="34" t="s">
-        <v>0</v>
-      </c>
+      <c r="B67" s="33"/>
       <c r="C67" s="21"/>
       <c r="D67" s="21"/>
       <c r="E67" s="21"/>
@@ -2879,9 +2886,7 @@
       <c r="H67" s="21"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B68" s="25" t="s">
-        <v>0</v>
-      </c>
+      <c r="B68" s="33"/>
       <c r="C68" s="21"/>
       <c r="D68" s="21"/>
       <c r="E68" s="21"/>
@@ -2890,9 +2895,7 @@
       <c r="H68" s="21"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B69" s="25" t="s">
-        <v>0</v>
-      </c>
+      <c r="B69" s="33"/>
       <c r="C69" s="21"/>
       <c r="D69" s="21"/>
       <c r="E69" s="21"/>
@@ -2901,9 +2904,7 @@
       <c r="H69" s="21"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B70" s="25" t="s">
-        <v>0</v>
-      </c>
+      <c r="B70" s="33"/>
       <c r="C70" s="21"/>
       <c r="D70" s="21"/>
       <c r="E70" s="21"/>
@@ -2912,9 +2913,7 @@
       <c r="H70" s="21"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B71" s="25" t="s">
-        <v>0</v>
-      </c>
+      <c r="B71" s="33"/>
       <c r="C71" s="21"/>
       <c r="D71" s="21"/>
       <c r="E71" s="21"/>
@@ -2923,9 +2922,7 @@
       <c r="H71" s="21"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B72" s="25" t="s">
-        <v>0</v>
-      </c>
+      <c r="B72" s="33"/>
       <c r="C72" s="21"/>
       <c r="D72" s="21"/>
       <c r="E72" s="21"/>
@@ -2934,9 +2931,7 @@
       <c r="H72" s="21"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B73" s="25" t="s">
-        <v>0</v>
-      </c>
+      <c r="B73" s="33"/>
       <c r="C73" s="21"/>
       <c r="D73" s="21"/>
       <c r="E73" s="21"/>
@@ -2945,9 +2940,7 @@
       <c r="H73" s="21"/>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B74" s="25" t="s">
-        <v>0</v>
-      </c>
+      <c r="B74" s="33"/>
       <c r="C74" s="21"/>
       <c r="D74" s="21"/>
       <c r="E74" s="21"/>
@@ -2956,9 +2949,7 @@
       <c r="H74" s="21"/>
     </row>
     <row r="75" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="25" t="s">
-        <v>0</v>
-      </c>
+      <c r="B75" s="33"/>
       <c r="C75" s="21"/>
       <c r="D75" s="21"/>
       <c r="E75" s="21"/>
@@ -3036,15 +3027,15 @@
       <c r="B84" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C84" s="28" t="s">
+      <c r="C84" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D84" s="29" t="s">
+      <c r="D84" s="27" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B85" s="25" t="s">
+      <c r="B85" s="24" t="s">
         <v>0</v>
       </c>
       <c r="C85" s="22" t="s">
@@ -3055,7 +3046,7 @@
       </c>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B86" s="25" t="s">
+      <c r="B86" s="24" t="s">
         <v>0</v>
       </c>
       <c r="C86" s="22" t="s">
@@ -3066,7 +3057,7 @@
       </c>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B87" s="25" t="s">
+      <c r="B87" s="24" t="s">
         <v>0</v>
       </c>
       <c r="C87" s="22" t="s">
@@ -3077,7 +3068,7 @@
       </c>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B88" s="25" t="s">
+      <c r="B88" s="24" t="s">
         <v>0</v>
       </c>
       <c r="C88" s="22" t="s">
@@ -3088,7 +3079,7 @@
       </c>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B89" s="25" t="s">
+      <c r="B89" s="24" t="s">
         <v>0</v>
       </c>
       <c r="C89" s="22" t="s">
@@ -3099,7 +3090,7 @@
       </c>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B90" s="25" t="s">
+      <c r="B90" s="24" t="s">
         <v>0</v>
       </c>
       <c r="C90" s="22" t="s">
@@ -3110,7 +3101,7 @@
       </c>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B91" s="23" t="s">
+      <c r="B91" s="30" t="s">
         <v>0</v>
       </c>
       <c r="C91" s="22" t="s">
@@ -3121,7 +3112,7 @@
       </c>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B92" s="23" t="s">
+      <c r="B92" s="30" t="s">
         <v>0</v>
       </c>
       <c r="C92" s="22" t="s">
@@ -3132,7 +3123,7 @@
       </c>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B93" s="23" t="s">
+      <c r="B93" s="30" t="s">
         <v>0</v>
       </c>
       <c r="C93" s="22" t="s">
@@ -3143,7 +3134,7 @@
       </c>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B94" s="23" t="s">
+      <c r="B94" s="30" t="s">
         <v>0</v>
       </c>
       <c r="C94" s="22" t="s">
@@ -3154,7 +3145,7 @@
       </c>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B95" s="23" t="s">
+      <c r="B95" s="30" t="s">
         <v>0</v>
       </c>
       <c r="C95" s="22" t="s">
@@ -3165,7 +3156,9 @@
       </c>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B96" s="27"/>
+      <c r="B96" s="24" t="s">
+        <v>0</v>
+      </c>
       <c r="C96" s="22" t="s">
         <v>100</v>
       </c>
@@ -3174,7 +3167,9 @@
       </c>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B97" s="27"/>
+      <c r="B97" s="24" t="s">
+        <v>0</v>
+      </c>
       <c r="C97" s="22" t="s">
         <v>101</v>
       </c>
@@ -3183,7 +3178,9 @@
       </c>
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B98" s="27"/>
+      <c r="B98" s="24" t="s">
+        <v>0</v>
+      </c>
       <c r="C98" s="22" t="s">
         <v>102</v>
       </c>
@@ -3192,7 +3189,9 @@
       </c>
     </row>
     <row r="99" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B99" s="27"/>
+      <c r="B99" s="24" t="s">
+        <v>0</v>
+      </c>
       <c r="C99" s="22" t="s">
         <v>103</v>
       </c>
@@ -3201,7 +3200,9 @@
       </c>
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B100" s="27"/>
+      <c r="B100" s="24" t="s">
+        <v>0</v>
+      </c>
       <c r="C100" s="22" t="s">
         <v>104</v>
       </c>
@@ -3210,7 +3211,9 @@
       </c>
     </row>
     <row r="101" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B101" s="27"/>
+      <c r="B101" s="24" t="s">
+        <v>0</v>
+      </c>
       <c r="C101" s="22" t="s">
         <v>105</v>
       </c>
@@ -3219,7 +3222,9 @@
       </c>
     </row>
     <row r="102" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B102" s="27"/>
+      <c r="B102" s="30" t="s">
+        <v>0</v>
+      </c>
       <c r="C102" s="22" t="s">
         <v>110</v>
       </c>
@@ -3228,7 +3233,9 @@
       </c>
     </row>
     <row r="103" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B103" s="27"/>
+      <c r="B103" s="30" t="s">
+        <v>0</v>
+      </c>
       <c r="C103" s="22" t="s">
         <v>111</v>
       </c>
@@ -3237,7 +3244,9 @@
       </c>
     </row>
     <row r="104" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B104" s="27"/>
+      <c r="B104" s="30" t="s">
+        <v>0</v>
+      </c>
       <c r="C104" s="22" t="s">
         <v>113</v>
       </c>
@@ -3246,8 +3255,10 @@
       </c>
     </row>
     <row r="105" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B105" s="27"/>
-      <c r="C105" s="30" t="s">
+      <c r="B105" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C105" s="28" t="s">
         <v>32</v>
       </c>
       <c r="D105" s="12" t="s">
@@ -3255,8 +3266,10 @@
       </c>
     </row>
     <row r="106" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B106" s="27"/>
-      <c r="C106" s="30" t="s">
+      <c r="B106" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C106" s="28" t="s">
         <v>34</v>
       </c>
       <c r="D106" s="12" t="s">
@@ -3264,8 +3277,10 @@
       </c>
     </row>
     <row r="107" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B107" s="27"/>
-      <c r="C107" s="30" t="s">
+      <c r="B107" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C107" s="28" t="s">
         <v>35</v>
       </c>
       <c r="D107" s="12" t="s">
@@ -3273,8 +3288,10 @@
       </c>
     </row>
     <row r="108" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B108" s="27"/>
-      <c r="C108" s="30" t="s">
+      <c r="B108" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C108" s="28" t="s">
         <v>36</v>
       </c>
       <c r="D108" s="12" t="s">
@@ -3283,8 +3300,10 @@
       <c r="F108" s="19"/>
     </row>
     <row r="109" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B109" s="27"/>
-      <c r="C109" s="30" t="s">
+      <c r="B109" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C109" s="28" t="s">
         <v>37</v>
       </c>
       <c r="D109" s="12" t="s">
@@ -3293,8 +3312,10 @@
       <c r="F109" s="19"/>
     </row>
     <row r="110" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B110" s="27"/>
-      <c r="C110" s="30" t="s">
+      <c r="B110" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C110" s="28" t="s">
         <v>38</v>
       </c>
       <c r="D110" s="12" t="s">
@@ -3303,8 +3324,10 @@
       <c r="F110" s="20"/>
     </row>
     <row r="111" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B111" s="27"/>
-      <c r="C111" s="30" t="s">
+      <c r="B111" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C111" s="28" t="s">
         <v>33</v>
       </c>
       <c r="D111" s="12" t="s">
@@ -3313,8 +3336,10 @@
       <c r="F111" s="21"/>
     </row>
     <row r="112" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B112" s="27"/>
-      <c r="C112" s="30" t="s">
+      <c r="B112" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C112" s="28" t="s">
         <v>39</v>
       </c>
       <c r="D112" s="12" t="s">
@@ -3323,8 +3348,10 @@
       <c r="F112" s="21"/>
     </row>
     <row r="113" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B113" s="27"/>
-      <c r="C113" s="30" t="s">
+      <c r="B113" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C113" s="28" t="s">
         <v>40</v>
       </c>
       <c r="D113" s="12" t="s">
@@ -3333,8 +3360,10 @@
       <c r="F113" s="21"/>
     </row>
     <row r="114" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B114" s="27"/>
-      <c r="C114" s="30" t="s">
+      <c r="B114" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C114" s="28" t="s">
         <v>41</v>
       </c>
       <c r="D114" s="12" t="s">
@@ -3343,8 +3372,10 @@
       <c r="F114" s="21"/>
     </row>
     <row r="115" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B115" s="27"/>
-      <c r="C115" s="30" t="s">
+      <c r="B115" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C115" s="28" t="s">
         <v>42</v>
       </c>
       <c r="D115" s="12" t="s">
@@ -3353,7 +3384,9 @@
       <c r="F115" s="19"/>
     </row>
     <row r="116" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B116" s="27"/>
+      <c r="B116" s="36" t="s">
+        <v>0</v>
+      </c>
       <c r="C116" s="18" t="s">
         <v>45</v>
       </c>
@@ -3363,7 +3396,9 @@
       <c r="F116" s="19"/>
     </row>
     <row r="117" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B117" s="27"/>
+      <c r="B117" s="36" t="s">
+        <v>0</v>
+      </c>
       <c r="C117" s="18" t="s">
         <v>46</v>
       </c>
@@ -3373,7 +3408,9 @@
       <c r="F117" s="19"/>
     </row>
     <row r="118" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B118" s="27"/>
+      <c r="B118" s="36" t="s">
+        <v>0</v>
+      </c>
       <c r="C118" s="18" t="s">
         <v>47</v>
       </c>
@@ -3383,7 +3420,9 @@
       <c r="F118" s="19"/>
     </row>
     <row r="119" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B119" s="27"/>
+      <c r="B119" s="36" t="s">
+        <v>0</v>
+      </c>
       <c r="C119" s="18" t="s">
         <v>48</v>
       </c>
@@ -3392,7 +3431,9 @@
       </c>
     </row>
     <row r="120" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B120" s="27"/>
+      <c r="B120" s="36" t="s">
+        <v>0</v>
+      </c>
       <c r="C120" s="18" t="s">
         <v>49</v>
       </c>
@@ -3401,7 +3442,9 @@
       </c>
     </row>
     <row r="121" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B121" s="27"/>
+      <c r="B121" s="36" t="s">
+        <v>0</v>
+      </c>
       <c r="C121" s="18" t="s">
         <v>50</v>
       </c>
@@ -3410,7 +3453,9 @@
       </c>
     </row>
     <row r="122" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B122" s="27"/>
+      <c r="B122" s="36" t="s">
+        <v>0</v>
+      </c>
       <c r="C122" s="18" t="s">
         <v>51</v>
       </c>
@@ -3419,7 +3464,9 @@
       </c>
     </row>
     <row r="123" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B123" s="27"/>
+      <c r="B123" s="36" t="s">
+        <v>0</v>
+      </c>
       <c r="C123" s="18" t="s">
         <v>52</v>
       </c>
@@ -3428,7 +3475,9 @@
       </c>
     </row>
     <row r="124" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B124" s="27"/>
+      <c r="B124" s="36" t="s">
+        <v>0</v>
+      </c>
       <c r="C124" s="18" t="s">
         <v>53</v>
       </c>
@@ -3437,7 +3486,9 @@
       </c>
     </row>
     <row r="125" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B125" s="27"/>
+      <c r="B125" s="36" t="s">
+        <v>0</v>
+      </c>
       <c r="C125" s="18" t="s">
         <v>54</v>
       </c>
@@ -3446,7 +3497,9 @@
       </c>
     </row>
     <row r="126" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B126" s="27"/>
+      <c r="B126" s="36" t="s">
+        <v>0</v>
+      </c>
       <c r="C126" s="18" t="s">
         <v>55</v>
       </c>
@@ -3455,7 +3508,9 @@
       </c>
     </row>
     <row r="127" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B127" s="27"/>
+      <c r="B127" s="36" t="s">
+        <v>0</v>
+      </c>
       <c r="C127" s="18" t="s">
         <v>56</v>
       </c>
@@ -3464,333 +3519,247 @@
       </c>
     </row>
     <row r="128" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B128" s="23" t="s">
-        <v>0</v>
-      </c>
+      <c r="B128" s="33"/>
       <c r="C128" s="20"/>
       <c r="D128" s="21"/>
     </row>
     <row r="129" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B129" s="23" t="s">
-        <v>0</v>
-      </c>
+      <c r="B129" s="33"/>
       <c r="C129" s="20"/>
       <c r="D129" s="21"/>
     </row>
     <row r="130" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B130" s="23" t="s">
-        <v>0</v>
-      </c>
+      <c r="B130" s="33"/>
       <c r="C130" s="20"/>
       <c r="D130" s="21"/>
     </row>
     <row r="131" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B131" s="23" t="s">
-        <v>0</v>
-      </c>
+      <c r="B131" s="33"/>
       <c r="C131" s="20"/>
       <c r="D131" s="21"/>
     </row>
     <row r="132" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B132" s="23" t="s">
-        <v>0</v>
-      </c>
+      <c r="B132" s="33"/>
       <c r="C132" s="20"/>
       <c r="D132" s="21"/>
     </row>
     <row r="133" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B133" s="23" t="s">
-        <v>0</v>
-      </c>
+      <c r="B133" s="33"/>
       <c r="C133" s="20"/>
       <c r="D133" s="21"/>
     </row>
     <row r="134" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B134" s="24" t="s">
-        <v>0</v>
-      </c>
+      <c r="B134" s="21"/>
       <c r="C134" s="21"/>
       <c r="D134" s="21"/>
     </row>
     <row r="135" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B135" s="24" t="s">
-        <v>0</v>
-      </c>
+      <c r="B135" s="21"/>
       <c r="C135" s="21"/>
       <c r="D135" s="21"/>
     </row>
     <row r="136" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B136" s="24" t="s">
-        <v>0</v>
-      </c>
+      <c r="B136" s="21"/>
       <c r="C136" s="21"/>
       <c r="D136" s="21"/>
     </row>
     <row r="137" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B137" s="24" t="s">
-        <v>0</v>
-      </c>
+      <c r="B137" s="21"/>
       <c r="C137" s="21"/>
       <c r="D137" s="21"/>
     </row>
     <row r="138" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B138" s="24" t="s">
-        <v>0</v>
-      </c>
+      <c r="B138" s="21"/>
       <c r="C138" s="21"/>
       <c r="D138" s="21"/>
     </row>
     <row r="139" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B139" s="24" t="s">
-        <v>0</v>
-      </c>
+      <c r="B139" s="21"/>
       <c r="C139" s="21"/>
       <c r="D139" s="21"/>
     </row>
     <row r="140" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B140" s="24" t="s">
-        <v>0</v>
-      </c>
+      <c r="B140" s="21"/>
       <c r="C140" s="21"/>
       <c r="D140" s="21"/>
     </row>
     <row r="141" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B141" s="24" t="s">
-        <v>0</v>
-      </c>
+      <c r="B141" s="21"/>
       <c r="C141" s="21"/>
       <c r="D141" s="21"/>
     </row>
     <row r="142" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B142" s="24" t="s">
-        <v>0</v>
-      </c>
+      <c r="B142" s="21"/>
       <c r="C142" s="21"/>
       <c r="D142" s="21"/>
     </row>
     <row r="143" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B143" s="24" t="s">
-        <v>0</v>
-      </c>
+      <c r="B143" s="21"/>
       <c r="C143" s="21"/>
       <c r="D143" s="21"/>
     </row>
     <row r="144" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B144" s="24" t="s">
-        <v>0</v>
-      </c>
+      <c r="B144" s="21"/>
       <c r="C144" s="21"/>
       <c r="D144" s="21"/>
     </row>
     <row r="145" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B145" s="24" t="s">
-        <v>0</v>
-      </c>
+      <c r="B145" s="21"/>
       <c r="C145" s="21"/>
       <c r="D145" s="21"/>
     </row>
     <row r="146" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B146" s="24" t="s">
-        <v>0</v>
-      </c>
+      <c r="B146" s="21"/>
       <c r="C146" s="21"/>
       <c r="D146" s="21"/>
     </row>
     <row r="147" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B147" s="24" t="s">
-        <v>0</v>
-      </c>
+      <c r="B147" s="21"/>
       <c r="C147" s="21"/>
       <c r="D147" s="21"/>
     </row>
     <row r="148" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B148" s="24" t="s">
-        <v>0</v>
-      </c>
+      <c r="B148" s="21"/>
       <c r="C148" s="21"/>
       <c r="D148" s="21"/>
     </row>
     <row r="149" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B149" s="24" t="s">
-        <v>0</v>
-      </c>
+      <c r="B149" s="21"/>
       <c r="C149" s="21"/>
       <c r="D149" s="21"/>
     </row>
     <row r="150" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B150" s="24" t="s">
-        <v>0</v>
-      </c>
+      <c r="B150" s="21"/>
       <c r="C150" s="21"/>
       <c r="D150" s="21"/>
     </row>
     <row r="151" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B151" s="24" t="s">
-        <v>0</v>
-      </c>
+      <c r="B151" s="21"/>
       <c r="C151" s="21"/>
       <c r="D151" s="21"/>
     </row>
     <row r="152" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B152" s="24" t="s">
-        <v>0</v>
-      </c>
+      <c r="B152" s="21"/>
       <c r="C152" s="21"/>
       <c r="D152" s="21"/>
     </row>
     <row r="153" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B153" s="20"/>
       <c r="C153" s="20"/>
       <c r="D153" s="20"/>
     </row>
     <row r="154" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B154" s="25" t="s">
-        <v>0</v>
-      </c>
+      <c r="B154" s="33"/>
       <c r="C154" s="21"/>
       <c r="D154" s="21"/>
     </row>
     <row r="155" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B155" s="25" t="s">
-        <v>0</v>
-      </c>
+      <c r="B155" s="33"/>
       <c r="C155" s="21"/>
       <c r="D155" s="21"/>
     </row>
     <row r="156" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B156" s="25" t="s">
-        <v>0</v>
-      </c>
+      <c r="B156" s="33"/>
       <c r="C156" s="21"/>
       <c r="D156" s="21"/>
     </row>
     <row r="157" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B157" s="25" t="s">
-        <v>0</v>
-      </c>
+      <c r="B157" s="33"/>
       <c r="C157" s="21"/>
       <c r="D157" s="21"/>
     </row>
     <row r="158" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B158" s="25" t="s">
-        <v>0</v>
-      </c>
+      <c r="B158" s="33"/>
       <c r="C158" s="21"/>
       <c r="D158" s="21"/>
     </row>
     <row r="159" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B159" s="25" t="s">
-        <v>0</v>
-      </c>
+      <c r="B159" s="33"/>
       <c r="C159" s="21"/>
       <c r="D159" s="21"/>
     </row>
     <row r="160" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B160" s="25" t="s">
-        <v>0</v>
-      </c>
+      <c r="B160" s="33"/>
       <c r="C160" s="21"/>
       <c r="D160" s="21"/>
     </row>
     <row r="161" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B161" s="25" t="s">
-        <v>0</v>
-      </c>
+      <c r="B161" s="33"/>
       <c r="C161" s="21"/>
       <c r="D161" s="21"/>
     </row>
     <row r="162" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B162" s="25" t="s">
-        <v>0</v>
-      </c>
+      <c r="B162" s="33"/>
       <c r="C162" s="21"/>
       <c r="D162" s="21"/>
     </row>
     <row r="163" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B163" s="25" t="s">
-        <v>0</v>
-      </c>
+      <c r="B163" s="33"/>
       <c r="C163" s="21"/>
       <c r="D163" s="21"/>
     </row>
     <row r="164" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B164" s="25" t="s">
-        <v>0</v>
-      </c>
+      <c r="B164" s="33"/>
       <c r="C164" s="21"/>
       <c r="D164" s="21"/>
     </row>
     <row r="165" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B165" s="25" t="s">
-        <v>0</v>
-      </c>
+      <c r="B165" s="33"/>
       <c r="C165" s="21"/>
       <c r="D165" s="21"/>
     </row>
     <row r="166" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B166" s="25" t="s">
-        <v>0</v>
-      </c>
+      <c r="B166" s="33"/>
       <c r="C166" s="21"/>
       <c r="D166" s="21"/>
     </row>
     <row r="167" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B167" s="25" t="s">
-        <v>0</v>
-      </c>
+      <c r="B167" s="33"/>
       <c r="C167" s="21"/>
       <c r="D167" s="21"/>
     </row>
     <row r="168" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B168" s="25" t="s">
-        <v>0</v>
-      </c>
+      <c r="B168" s="33"/>
       <c r="C168" s="21"/>
       <c r="D168" s="21"/>
     </row>
     <row r="169" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B169" s="25" t="s">
-        <v>0</v>
-      </c>
+      <c r="B169" s="33"/>
       <c r="C169" s="21"/>
       <c r="D169" s="21"/>
     </row>
     <row r="170" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B170" s="25" t="s">
-        <v>0</v>
-      </c>
+      <c r="B170" s="33"/>
       <c r="C170" s="21"/>
       <c r="D170" s="21"/>
     </row>
     <row r="171" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B171" s="25" t="s">
-        <v>0</v>
-      </c>
+      <c r="B171" s="33"/>
       <c r="C171" s="21"/>
       <c r="D171" s="21"/>
     </row>
     <row r="172" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B172" s="25" t="s">
-        <v>0</v>
-      </c>
+      <c r="B172" s="33"/>
       <c r="C172" s="21"/>
       <c r="D172" s="21"/>
     </row>
     <row r="173" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B173" s="25" t="s">
-        <v>0</v>
-      </c>
+      <c r="B173" s="33"/>
       <c r="C173" s="21"/>
       <c r="D173" s="21"/>
     </row>
     <row r="174" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B174" s="20"/>
       <c r="C174" s="20"/>
       <c r="D174" s="21"/>
     </row>
     <row r="175" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B175" s="20"/>
       <c r="C175" s="20"/>
       <c r="D175" s="21"/>
     </row>
     <row r="176" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B176" s="20"/>
       <c r="C176" s="20"/>
       <c r="D176" s="21"/>
     </row>
@@ -3875,8 +3844,8 @@
       <c r="D196" s="21"/>
     </row>
     <row r="197" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C197" s="26"/>
-      <c r="D197" s="26"/>
+      <c r="C197" s="25"/>
+      <c r="D197" s="25"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Fix Error Tree 1
Former-commit-id: 268ee7bb4f1da9b8bcd960f789aaaa6c36f94b98
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Clustering.xlsx
+++ b/Docs/Content/HungryDragonContent_Clustering.xlsx
@@ -344,9 +344,6 @@
     <t>CLUSTER_TREE_001_RULE_017</t>
   </si>
   <si>
-    <t>model.deviceProfile &lt;= 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">['GROUP_6','GROUP_7'].indexOf(model.countryGroup) &gt;=0 </t>
   </si>
   <si>
@@ -465,6 +462,9 @@
   </si>
   <si>
     <t>model.shopEntered</t>
+  </si>
+  <si>
+    <t>model.deviceProfile &gt;= 2</t>
   </si>
 </sst>
 </file>
@@ -1843,8 +1843,8 @@
   </sheetPr>
   <dimension ref="A3:K197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H66" sqref="H66"/>
+    <sheetView tabSelected="1" topLeftCell="C79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2127,10 +2127,10 @@
         <v>29</v>
       </c>
       <c r="E27" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="F27" s="12" t="s">
         <v>116</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>117</v>
       </c>
       <c r="G27" s="12"/>
       <c r="H27" s="12"/>
@@ -2146,7 +2146,7 @@
         <v>30</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F28" s="12"/>
       <c r="G28" s="12"/>
@@ -2165,7 +2165,7 @@
         <v>31</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
@@ -2178,16 +2178,16 @@
         <v>0</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>93</v>
       </c>
       <c r="E30" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="F30" s="12" t="s">
         <v>120</v>
-      </c>
-      <c r="F30" s="12" t="s">
-        <v>121</v>
       </c>
       <c r="G30" s="12"/>
       <c r="H30" s="12"/>
@@ -2197,14 +2197,14 @@
         <v>0</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D31" s="12" t="s">
         <v>94</v>
       </c>
       <c r="E31" s="12"/>
       <c r="F31" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G31" s="12" t="s">
         <v>24</v>
@@ -2216,14 +2216,14 @@
         <v>0</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D32" s="12" t="s">
         <v>95</v>
       </c>
       <c r="E32" s="12"/>
       <c r="F32" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G32" s="12" t="s">
         <v>24</v>
@@ -2235,14 +2235,14 @@
         <v>0</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D33" s="12" t="s">
         <v>96</v>
       </c>
       <c r="E33" s="12"/>
       <c r="F33" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G33" s="12" t="s">
         <v>23</v>
@@ -2254,14 +2254,14 @@
         <v>0</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>97</v>
       </c>
       <c r="E34" s="12"/>
       <c r="F34" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G34" s="12" t="s">
         <v>24</v>
@@ -2273,16 +2273,16 @@
         <v>0</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D35" s="12" t="s">
         <v>100</v>
       </c>
       <c r="E35" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="F35" s="12" t="s">
         <v>126</v>
-      </c>
-      <c r="F35" s="12" t="s">
-        <v>127</v>
       </c>
       <c r="G35" s="12"/>
       <c r="H35" s="12"/>
@@ -2292,7 +2292,7 @@
         <v>0</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D36" s="12" t="s">
         <v>101</v>
@@ -2311,7 +2311,7 @@
         <v>0</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>102</v>
@@ -2330,7 +2330,7 @@
         <v>0</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D38" s="12" t="s">
         <v>103</v>
@@ -2349,14 +2349,14 @@
         <v>0</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D39" s="12" t="s">
         <v>104</v>
       </c>
       <c r="E39" s="12"/>
       <c r="F39" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G39" s="12" t="s">
         <v>24</v>
@@ -2368,14 +2368,14 @@
         <v>0</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D40" s="12" t="s">
         <v>105</v>
       </c>
       <c r="E40" s="12"/>
       <c r="F40" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G40" s="12" t="s">
         <v>24</v>
@@ -2387,10 +2387,10 @@
         <v>0</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
@@ -2406,10 +2406,10 @@
         <v>0</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E42" s="12"/>
       <c r="F42" s="12"/>
@@ -2425,10 +2425,10 @@
         <v>0</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E43" s="12"/>
       <c r="F43" s="12"/>
@@ -3086,7 +3086,7 @@
         <v>30</v>
       </c>
       <c r="D89" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.25">
@@ -3174,7 +3174,7 @@
         <v>101</v>
       </c>
       <c r="D97" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.25">
@@ -3185,7 +3185,7 @@
         <v>102</v>
       </c>
       <c r="D98" s="12" t="s">
-        <v>106</v>
+        <v>146</v>
       </c>
     </row>
     <row r="99" spans="2:6" x14ac:dyDescent="0.25">
@@ -3196,7 +3196,7 @@
         <v>103</v>
       </c>
       <c r="D99" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.25">
@@ -3207,7 +3207,7 @@
         <v>104</v>
       </c>
       <c r="D100" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="101" spans="2:6" x14ac:dyDescent="0.25">
@@ -3218,7 +3218,7 @@
         <v>105</v>
       </c>
       <c r="D101" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="102" spans="2:6" x14ac:dyDescent="0.25">
@@ -3226,10 +3226,10 @@
         <v>0</v>
       </c>
       <c r="C102" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D102" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="103" spans="2:6" x14ac:dyDescent="0.25">
@@ -3237,10 +3237,10 @@
         <v>0</v>
       </c>
       <c r="C103" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D103" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="104" spans="2:6" x14ac:dyDescent="0.25">
@@ -3248,10 +3248,10 @@
         <v>0</v>
       </c>
       <c r="C104" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D104" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="105" spans="2:6" x14ac:dyDescent="0.25">
@@ -3295,7 +3295,7 @@
         <v>36</v>
       </c>
       <c r="D108" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F108" s="19"/>
     </row>
@@ -3307,7 +3307,7 @@
         <v>37</v>
       </c>
       <c r="D109" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F109" s="19"/>
     </row>
@@ -3319,7 +3319,7 @@
         <v>38</v>
       </c>
       <c r="D110" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F110" s="20"/>
     </row>
@@ -3331,7 +3331,7 @@
         <v>33</v>
       </c>
       <c r="D111" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F111" s="21"/>
     </row>
@@ -3343,7 +3343,7 @@
         <v>39</v>
       </c>
       <c r="D112" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F112" s="21"/>
     </row>
@@ -3355,7 +3355,7 @@
         <v>40</v>
       </c>
       <c r="D113" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F113" s="21"/>
     </row>
@@ -3367,7 +3367,7 @@
         <v>41</v>
       </c>
       <c r="D114" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F114" s="21"/>
     </row>
@@ -3379,7 +3379,7 @@
         <v>42</v>
       </c>
       <c r="D115" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F115" s="19"/>
     </row>
@@ -3427,7 +3427,7 @@
         <v>48</v>
       </c>
       <c r="D119" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="120" spans="2:6" x14ac:dyDescent="0.25">
@@ -3449,7 +3449,7 @@
         <v>50</v>
       </c>
       <c r="D121" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="122" spans="2:6" x14ac:dyDescent="0.25">
@@ -3460,7 +3460,7 @@
         <v>51</v>
       </c>
       <c r="D122" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="123" spans="2:6" x14ac:dyDescent="0.25">
@@ -3471,7 +3471,7 @@
         <v>52</v>
       </c>
       <c r="D123" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="124" spans="2:6" x14ac:dyDescent="0.25">
@@ -3482,7 +3482,7 @@
         <v>53</v>
       </c>
       <c r="D124" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="125" spans="2:6" x14ac:dyDescent="0.25">
@@ -3504,7 +3504,7 @@
         <v>55</v>
       </c>
       <c r="D126" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="127" spans="2:6" x14ac:dyDescent="0.25">
@@ -3515,7 +3515,7 @@
         <v>56</v>
       </c>
       <c r="D127" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="128" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Decimal point error in R trees fix
Former-commit-id: 44201a9d1c8c68e145f6a71caa33865aa3dfb057
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Clustering.xlsx
+++ b/Docs/Content/HungryDragonContent_Clustering.xlsx
@@ -293,9 +293,6 @@
     <t>['GROUP_1','GROUP_2','GROUP_3','GROUP_4'].indexOf(model.countryGroup) &gt;= 0</t>
   </si>
   <si>
-    <t>model.score &gt;= 10e+3</t>
-  </si>
-  <si>
     <t>model.deviceProfile != 0</t>
   </si>
   <si>
@@ -359,9 +356,6 @@
     <t>CLUSTER_TREE_001_RULE_019</t>
   </si>
   <si>
-    <t>model.score &gt;= 41e+3</t>
-  </si>
-  <si>
     <t>CLUSTER_TREE_001_RULE_020</t>
   </si>
   <si>
@@ -416,15 +410,6 @@
     <t>model.deviceProfile &lt;= 2</t>
   </si>
   <si>
-    <t>model.score &gt;= 21e+3</t>
-  </si>
-  <si>
-    <t>model.score &gt;= 23e+3</t>
-  </si>
-  <si>
-    <t>model.score &gt;= 17e+3</t>
-  </si>
-  <si>
     <t>['Amazon','Asus','Google','Huawei','ipad','ipod','Lenovo','Lge','OnePlus','Samsung','Sony'].indexOf(model.modelGroup) &gt;= 0</t>
   </si>
   <si>
@@ -446,9 +431,6 @@
     <t>model.score &gt;= 7676</t>
   </si>
   <si>
-    <t>model.score &gt;= 11e+3</t>
-  </si>
-  <si>
     <t>model.maxProgression &gt;= 106</t>
   </si>
   <si>
@@ -465,6 +447,24 @@
   </si>
   <si>
     <t>model.deviceProfile &gt;= 2</t>
+  </si>
+  <si>
+    <t>model.score &gt;= 10,41e+3</t>
+  </si>
+  <si>
+    <t>model.score &gt;= 40,91e+3</t>
+  </si>
+  <si>
+    <t>model.score &gt;= 21,39e+3</t>
+  </si>
+  <si>
+    <t>model.score &gt;= 23,15e+3</t>
+  </si>
+  <si>
+    <t>model.score &gt;= 16,59e+3</t>
+  </si>
+  <si>
+    <t>model.score &gt;= 10,86e+3</t>
   </si>
 </sst>
 </file>
@@ -1843,8 +1843,8 @@
   </sheetPr>
   <dimension ref="A3:K197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D104" sqref="D104"/>
+    <sheetView tabSelected="1" topLeftCell="C85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D126" sqref="D126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2127,10 +2127,10 @@
         <v>29</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G27" s="12"/>
       <c r="H27" s="12"/>
@@ -2146,7 +2146,7 @@
         <v>30</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F28" s="12"/>
       <c r="G28" s="12"/>
@@ -2165,7 +2165,7 @@
         <v>31</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
@@ -2178,16 +2178,16 @@
         <v>0</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G30" s="12"/>
       <c r="H30" s="12"/>
@@ -2197,14 +2197,14 @@
         <v>0</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E31" s="12"/>
       <c r="F31" s="12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G31" s="12" t="s">
         <v>24</v>
@@ -2216,14 +2216,14 @@
         <v>0</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E32" s="12"/>
       <c r="F32" s="12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G32" s="12" t="s">
         <v>24</v>
@@ -2235,14 +2235,14 @@
         <v>0</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E33" s="12"/>
       <c r="F33" s="12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G33" s="12" t="s">
         <v>23</v>
@@ -2254,14 +2254,14 @@
         <v>0</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E34" s="12"/>
       <c r="F34" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G34" s="12" t="s">
         <v>24</v>
@@ -2273,16 +2273,16 @@
         <v>0</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G35" s="12"/>
       <c r="H35" s="12"/>
@@ -2292,10 +2292,10 @@
         <v>0</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
@@ -2311,10 +2311,10 @@
         <v>0</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
@@ -2330,10 +2330,10 @@
         <v>0</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E38" s="12"/>
       <c r="F38" s="12"/>
@@ -2349,14 +2349,14 @@
         <v>0</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E39" s="12"/>
       <c r="F39" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G39" s="12" t="s">
         <v>24</v>
@@ -2368,14 +2368,14 @@
         <v>0</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E40" s="12"/>
       <c r="F40" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G40" s="12" t="s">
         <v>24</v>
@@ -2387,10 +2387,10 @@
         <v>0</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
@@ -2406,10 +2406,10 @@
         <v>0</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E42" s="12"/>
       <c r="F42" s="12"/>
@@ -2425,10 +2425,10 @@
         <v>0</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E43" s="12"/>
       <c r="F43" s="12"/>
@@ -3053,7 +3053,7 @@
         <v>27</v>
       </c>
       <c r="D86" s="12" t="s">
-        <v>89</v>
+        <v>141</v>
       </c>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.25">
@@ -3064,7 +3064,7 @@
         <v>28</v>
       </c>
       <c r="D87" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.25">
@@ -3075,7 +3075,7 @@
         <v>29</v>
       </c>
       <c r="D88" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.25">
@@ -3086,7 +3086,7 @@
         <v>30</v>
       </c>
       <c r="D89" s="12" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.25">
@@ -3097,7 +3097,7 @@
         <v>31</v>
       </c>
       <c r="D90" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.25">
@@ -3105,10 +3105,10 @@
         <v>0</v>
       </c>
       <c r="C91" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D91" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.25">
@@ -3116,10 +3116,10 @@
         <v>0</v>
       </c>
       <c r="C92" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D92" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.25">
@@ -3127,10 +3127,10 @@
         <v>0</v>
       </c>
       <c r="C93" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D93" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.25">
@@ -3138,10 +3138,10 @@
         <v>0</v>
       </c>
       <c r="C94" s="22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D94" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.25">
@@ -3149,7 +3149,7 @@
         <v>0</v>
       </c>
       <c r="C95" s="22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D95" s="12" t="s">
         <v>58</v>
@@ -3160,7 +3160,7 @@
         <v>0</v>
       </c>
       <c r="C96" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D96" s="12" t="s">
         <v>57</v>
@@ -3171,10 +3171,10 @@
         <v>0</v>
       </c>
       <c r="C97" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D97" s="12" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.25">
@@ -3182,10 +3182,10 @@
         <v>0</v>
       </c>
       <c r="C98" s="22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D98" s="12" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="99" spans="2:6" x14ac:dyDescent="0.25">
@@ -3193,10 +3193,10 @@
         <v>0</v>
       </c>
       <c r="C99" s="22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D99" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.25">
@@ -3204,10 +3204,10 @@
         <v>0</v>
       </c>
       <c r="C100" s="22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D100" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="101" spans="2:6" x14ac:dyDescent="0.25">
@@ -3215,10 +3215,10 @@
         <v>0</v>
       </c>
       <c r="C101" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D101" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="102" spans="2:6" x14ac:dyDescent="0.25">
@@ -3226,10 +3226,10 @@
         <v>0</v>
       </c>
       <c r="C102" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D102" s="12" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
     </row>
     <row r="103" spans="2:6" x14ac:dyDescent="0.25">
@@ -3237,10 +3237,10 @@
         <v>0</v>
       </c>
       <c r="C103" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D103" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="104" spans="2:6" x14ac:dyDescent="0.25">
@@ -3248,10 +3248,10 @@
         <v>0</v>
       </c>
       <c r="C104" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="D104" s="12" t="s">
         <v>112</v>
-      </c>
-      <c r="D104" s="12" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="105" spans="2:6" x14ac:dyDescent="0.25">
@@ -3273,7 +3273,7 @@
         <v>34</v>
       </c>
       <c r="D106" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="107" spans="2:6" x14ac:dyDescent="0.25">
@@ -3284,7 +3284,7 @@
         <v>35</v>
       </c>
       <c r="D107" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="108" spans="2:6" x14ac:dyDescent="0.25">
@@ -3295,7 +3295,7 @@
         <v>36</v>
       </c>
       <c r="D108" s="12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F108" s="19"/>
     </row>
@@ -3307,7 +3307,7 @@
         <v>37</v>
       </c>
       <c r="D109" s="12" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="F109" s="19"/>
     </row>
@@ -3319,7 +3319,7 @@
         <v>38</v>
       </c>
       <c r="D110" s="12" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="F110" s="20"/>
     </row>
@@ -3331,7 +3331,7 @@
         <v>33</v>
       </c>
       <c r="D111" s="12" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="F111" s="21"/>
     </row>
@@ -3343,7 +3343,7 @@
         <v>39</v>
       </c>
       <c r="D112" s="12" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="F112" s="21"/>
     </row>
@@ -3355,7 +3355,7 @@
         <v>40</v>
       </c>
       <c r="D113" s="12" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F113" s="21"/>
     </row>
@@ -3367,7 +3367,7 @@
         <v>41</v>
       </c>
       <c r="D114" s="12" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F114" s="21"/>
     </row>
@@ -3379,7 +3379,7 @@
         <v>42</v>
       </c>
       <c r="D115" s="12" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F115" s="19"/>
     </row>
@@ -3403,7 +3403,7 @@
         <v>46</v>
       </c>
       <c r="D117" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F117" s="19"/>
     </row>
@@ -3415,7 +3415,7 @@
         <v>47</v>
       </c>
       <c r="D118" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F118" s="19"/>
     </row>
@@ -3427,7 +3427,7 @@
         <v>48</v>
       </c>
       <c r="D119" s="12" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="120" spans="2:6" x14ac:dyDescent="0.25">
@@ -3438,7 +3438,7 @@
         <v>49</v>
       </c>
       <c r="D120" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="121" spans="2:6" x14ac:dyDescent="0.25">
@@ -3449,7 +3449,7 @@
         <v>50</v>
       </c>
       <c r="D121" s="12" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
     </row>
     <row r="122" spans="2:6" x14ac:dyDescent="0.25">
@@ -3460,7 +3460,7 @@
         <v>51</v>
       </c>
       <c r="D122" s="12" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="123" spans="2:6" x14ac:dyDescent="0.25">
@@ -3471,7 +3471,7 @@
         <v>52</v>
       </c>
       <c r="D123" s="12" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="124" spans="2:6" x14ac:dyDescent="0.25">
@@ -3482,7 +3482,7 @@
         <v>53</v>
       </c>
       <c r="D124" s="12" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="125" spans="2:6" x14ac:dyDescent="0.25">
@@ -3493,7 +3493,7 @@
         <v>54</v>
       </c>
       <c r="D125" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="126" spans="2:6" x14ac:dyDescent="0.25">
@@ -3504,7 +3504,7 @@
         <v>55</v>
       </c>
       <c r="D126" s="12" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="127" spans="2:6" x14ac:dyDescent="0.25">
@@ -3515,7 +3515,7 @@
         <v>56</v>
       </c>
       <c r="D127" s="12" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="128" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix scientific notation in rules
Former-commit-id: e9abed264b1ec1642341347e36ce12434bcc8062
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Clustering.xlsx
+++ b/Docs/Content/HungryDragonContent_Clustering.xlsx
@@ -449,22 +449,22 @@
     <t>model.deviceProfile &gt;= 2</t>
   </si>
   <si>
-    <t>model.score &gt;= 10,41e+3</t>
-  </si>
-  <si>
-    <t>model.score &gt;= 40,91e+3</t>
-  </si>
-  <si>
-    <t>model.score &gt;= 21,39e+3</t>
-  </si>
-  <si>
-    <t>model.score &gt;= 23,15e+3</t>
-  </si>
-  <si>
-    <t>model.score &gt;= 16,59e+3</t>
-  </si>
-  <si>
-    <t>model.score &gt;= 10,86e+3</t>
+    <t>model.score &gt;= 1041e+1</t>
+  </si>
+  <si>
+    <t>model.score &gt;= 4091e+1</t>
+  </si>
+  <si>
+    <t>model.score &gt;= 2139e+1</t>
+  </si>
+  <si>
+    <t>model.score &gt;= 2315e+1</t>
+  </si>
+  <si>
+    <t>model.score &gt;= 1659e+1</t>
+  </si>
+  <si>
+    <t>model.score &gt;= 1086e+1</t>
   </si>
 </sst>
 </file>
@@ -1844,7 +1844,7 @@
   <dimension ref="A3:K197"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D126" sqref="D126"/>
+      <selection activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fix tree update 07/09
Former-commit-id: 8cd42d79d12b42ffa254bf0119d3ad7d51562301
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Clustering.xlsx
+++ b/Docs/Content/HungryDragonContent_Clustering.xlsx
@@ -341,9 +341,6 @@
     <t>model.score &gt;= 5753</t>
   </si>
   <si>
-    <t>model.score &gt;= 8262</t>
-  </si>
-  <si>
     <t>model.score &gt;= 8808</t>
   </si>
   <si>
@@ -351,6 +348,9 @@
   </si>
   <si>
     <t>model.score &gt;= 14.46e+3</t>
+  </si>
+  <si>
+    <t>model.score &gt;= 8282</t>
   </si>
 </sst>
 </file>
@@ -1793,8 +1793,8 @@
   </sheetPr>
   <dimension ref="A3:K185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C103" sqref="C103"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2982,7 +2982,7 @@
         <v>34</v>
       </c>
       <c r="D93" s="12" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.25">
@@ -3026,7 +3026,7 @@
         <v>38</v>
       </c>
       <c r="D97" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.25">
@@ -3140,7 +3140,7 @@
         <v>47</v>
       </c>
       <c r="D109" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F109" s="21"/>
     </row>
@@ -3176,7 +3176,7 @@
         <v>50</v>
       </c>
       <c r="D112" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F112" s="19"/>
     </row>

</xml_diff>